<commit_message>
Update the list of nemo variables in the pre basic identifiedmissing file with the shaconemo repository 204.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="271">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -692,6 +692,12 @@
   </si>
   <si>
     <t xml:space="preserve">tasLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by either LPJ-GUESS or H-TESSEL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind &amp; Andrea Alessandri</t>
   </si>
   <si>
     <t xml:space="preserve">tslsiLut</t>
@@ -946,8 +952,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F99" activeCellId="0" sqref="F99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B174" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C191" activeCellId="0" sqref="C191:C404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -955,7 +961,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="97.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.71"/>
@@ -2858,98 +2864,98 @@
         <v>223</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="F145" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F145" s="0" t="s">
-        <v>217</v>
-      </c>
       <c r="G145" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F146" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="G146" s="0" t="s">
         <v>225</v>
-      </c>
-      <c r="F146" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="G146" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F147" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G147" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F148" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F149" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G149" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F150" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G150" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F151" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G151" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F152" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="G152" s="0" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2957,7 +2963,7 @@
         <v>117</v>
       </c>
       <c r="F153" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G153" s="0" t="s">
         <v>112</v>
@@ -2968,7 +2974,7 @@
         <v>121</v>
       </c>
       <c r="F154" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G154" s="0" t="s">
         <v>112</v>
@@ -2976,7 +2982,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F155" s="0" t="s">
         <v>181</v>
@@ -2987,7 +2993,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F156" s="0" t="s">
         <v>128</v>
@@ -2998,7 +3004,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F157" s="0" t="s">
         <v>128</v>
@@ -3009,7 +3015,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F158" s="0" t="s">
         <v>128</v>
@@ -3020,7 +3026,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F159" s="0" t="s">
         <v>128</v>
@@ -3031,7 +3037,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F160" s="0" t="s">
         <v>128</v>
@@ -3042,7 +3048,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F161" s="0" t="s">
         <v>128</v>
@@ -3053,7 +3059,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F162" s="0" t="s">
         <v>128</v>
@@ -3064,7 +3070,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F163" s="0" t="s">
         <v>128</v>
@@ -3075,7 +3081,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F164" s="0" t="s">
         <v>128</v>
@@ -3086,7 +3092,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G166" s="0" t="s">
         <v>112</v>
@@ -3094,7 +3100,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F168" s="0" t="s">
         <v>120</v>
@@ -3105,10 +3111,10 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F169" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G169" s="0" t="s">
         <v>112</v>
@@ -3116,10 +3122,10 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F170" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G170" s="0" t="s">
         <v>112</v>
@@ -3127,10 +3133,10 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F171" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G171" s="0" t="s">
         <v>112</v>
@@ -3138,10 +3144,10 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F172" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G172" s="0" t="s">
         <v>112</v>
@@ -3149,10 +3155,10 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F173" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G173" s="0" t="s">
         <v>112</v>
@@ -3160,7 +3166,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F174" s="0" t="s">
         <v>157</v>
@@ -3171,7 +3177,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F175" s="0" t="s">
         <v>157</v>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F176" s="0" t="s">
         <v>157</v>
@@ -3193,7 +3199,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F177" s="0" t="s">
         <v>157</v>
@@ -3204,7 +3210,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C178" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F178" s="0" t="s">
         <v>157</v>
@@ -3215,7 +3221,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F179" s="0" t="s">
         <v>157</v>
@@ -3226,10 +3232,10 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F180" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G180" s="0" t="s">
         <v>112</v>
@@ -3237,10 +3243,10 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F181" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="G181" s="0" t="s">
         <v>112</v>
@@ -3248,7 +3254,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F182" s="0" t="s">
         <v>157</v>
@@ -3259,7 +3265,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F183" s="0" t="s">
         <v>157</v>
@@ -3270,7 +3276,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F184" s="0" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
Adding variables to the pre basic ignored and pre basic identified missing files, update for ping files in shaconemo revision 210
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="287">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -833,6 +833,54 @@
   </si>
   <si>
     <t xml:space="preserve">nppRoot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available inLPJ-GUESS. Not available in PISCES, which means not available in NEMO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind, Raffaele Bernardello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dissicabio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in PISCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raffaele Bernardello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dissi13c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phabio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fg13co2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dissicabioos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dissi13cos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o2satos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eparag100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spco2abio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sisnconc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in PISCES. Not available in LIM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raffaele Bernardello, David Docquier, Thomas Reerink</t>
   </si>
 </sst>
 </file>
@@ -842,7 +890,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -872,6 +920,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -916,7 +975,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -930,6 +989,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -952,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B174" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C191" activeCellId="0" sqref="C191:C404"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F226" activeCellId="0" sqref="F226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,6 +3352,273 @@
         <v>112</v>
       </c>
     </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C186" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G186" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C187" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G187" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C188" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G188" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C189" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G189" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C190" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G190" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C191" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G191" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C192" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G192" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C193" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G193" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C195" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G195" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C196" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G196" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C197" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G197" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C198" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F198" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G198" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C199" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G199" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C200" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F200" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G200" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F215" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G215" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C216" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F216" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G216" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C217" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G217" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="F218" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G218" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C219" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F219" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G219" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C220" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F220" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G220" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C221" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F221" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G221" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="F222" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G222" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C223" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="F223" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G223" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C225" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F225" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="G225" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Reorder the "same as" LPJ_GUESS variables, so they are in one block - they might go to available vars after check and discussion
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="286">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -373,309 +373,426 @@
     <t xml:space="preserve">Can not be produced by LPJ-GUESS: Finest timestep in LPJ-GUESS is day, so RH is already reported on that timestep</t>
   </si>
   <si>
+    <t xml:space="preserve">mrsfl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No frozen fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegHeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: As only trees have a height in LPJ-GUESS, vegHeightTree in Emon is the only height variable reported.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co23D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilAbove1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Only have total soil C, no layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilBelow1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c14Veg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No isotopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c14Litter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c14Soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c13Veg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c13Litter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c13Soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c13Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rac14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhc13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dissi14c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrlso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fNVegSoil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No process that goes directly from veg to soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wtd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not calculated in this version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrtws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Don't have water stirage for anything else than for soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cVegTree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Don't seperate natural vegetation in vegetation type tiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cVegShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cVegGrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cLitterTree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cLitterShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cLitterGrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilTree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilGrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilLevels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoilPools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Too much work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tSoilPools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fVegLitterSenescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fVegLitterMortality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fVegSoilSenescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fVegSoilMortality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nppStem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nppOther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gppShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No shrubs in this version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nppShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhTree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Can't seperate rh between vegetation types as they compete for the same space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhGrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegHeightGrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: grass doesn't have a height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegHeightShrub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegHeightCrop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: crop doesn't have a height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegHeightPasture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetlandCH4prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not in this version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetlandCH4cons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fN2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fNOx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoomicro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Pisces?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoomeso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoomisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppdiat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppdiaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppcalc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pppico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppmisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expfe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expcalc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exparag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fgdms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fgco2nat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fgco2abio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fg14co2abio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fddtdic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fddtdin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fddtdip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fddtdife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fddtdisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fddtalk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbddtdic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbddtdin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbddtdip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbddtdife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbddtdisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbddtalk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: H-TESSEL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cMisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Don't have this in LPJ-GUESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tasLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by either LPJ-GUESS or H-TESSEL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind &amp; Andrea Alessandri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tslsiLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hussLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hflsLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfssLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsusLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlusLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sweLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fahLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Only tree that has a height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetlandFrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c14Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetlandCH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gppc14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhc14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">netAtmosLandC14Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gppc13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rac13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">netAtmosLandC13Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fg14co2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zfullo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrfso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burntFractionAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not calculated in LPJ-GUESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fVegSoil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No process that does this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treeFracPrimDec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treeFracPrimEver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treeFracSecDec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treeFracSecEver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c3PftFrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c4PftFrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nppLeaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nppWood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nppRoot</t>
+  </si>
+  <si>
     <t xml:space="preserve">mrsll</t>
   </si>
   <si>
     <t xml:space="preserve">Can not be produced by LPJ-GUESS: No frozen fraction of water, so same as mrsol</t>
   </si>
   <si>
-    <t xml:space="preserve">mrsfl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No frozen fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegHeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: As only trees have a height in LPJ-GUESS, vegHeightTree in Emon is the only height variable reported.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">co23D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilAbove1m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Only have total soil C, no layers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilBelow1m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c14Veg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No isotopes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c14Litter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c14Soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c13Veg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c13Litter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c13Soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c13Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rac14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhc13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dissi14c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrlso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fNVegSoil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No process that goes directly from veg to soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wtd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not calculated in this version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrtws</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Don't have water stirage for anything else than for soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cVegTree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Don't seperate natural vegetation in vegetation type tiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cVegShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cVegGrass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cLitterTree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cLitterShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cLitterGrass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilTree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilGrass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilLevels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cSoilPools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Too much work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tSoilPools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fVegLitterSenescence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fVegLitterMortality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fVegSoilSenescence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fVegSoilMortality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nppStem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nppOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gppShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No shrubs in this version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nppShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhTree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Can't seperate rh between vegetation types as they compete for the same space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhGrass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegHeightGrass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: grass doesn't have a height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegHeightShrub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegHeightCrop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: crop doesn't have a height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegHeightPasture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wetlandCH4prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not in this version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wetlandCH4cons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fN2O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fNOx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoomicro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Pisces?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoomeso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoomisc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppdiat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppdiaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppcalc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pppico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppmisc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expfe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expsi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expcalc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exparag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fgdms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fgco2nat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fgco2abio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fg14co2abio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fddtdic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fddtdin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fddtdip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fddtdife</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fddtdisi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fddtalk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbddtdic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbddtdin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbddtdip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbddtdife</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbddtdisi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbddtalk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: H-TESSEL?</t>
-  </si>
-  <si>
     <t xml:space="preserve">netAtmosLandCO2Flux</t>
   </si>
   <si>
@@ -685,105 +802,12 @@
     <t xml:space="preserve">nep</t>
   </si>
   <si>
-    <t xml:space="preserve">cMisc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Don't have this in LPJ-GUESS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by either LPJ-GUESS or H-TESSEL.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Warlind &amp; Andrea Alessandri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tslsiLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hussLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hflsLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hfssLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsusLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlusLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sweLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fahLut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Same as mrsol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Only tree that has a height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wetlandFrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c14Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wetlandCH4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gppc14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhc14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">netAtmosLandC14Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gppc13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rac13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">netAtmosLandC13Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fg14co2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zfullo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrfso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">burntFractionAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: Not calculated in LPJ-GUESS</t>
-  </si>
-  <si>
     <t xml:space="preserve">fFire</t>
   </si>
   <si>
     <t xml:space="preserve">Can not be produced by LPJ-GUESS: Same as fFireNat</t>
   </si>
   <si>
-    <t xml:space="preserve">fVegSoil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can not be produced by LPJ-GUESS: No process that does this</t>
-  </si>
-  <si>
     <t xml:space="preserve">fHarvest</t>
   </si>
   <si>
@@ -796,24 +820,6 @@
     <t xml:space="preserve">Can not be produced by LPJ-GUESS: Same as cLitterCwd</t>
   </si>
   <si>
-    <t xml:space="preserve">treeFracPrimDec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treeFracPrimEver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treeFracSecDec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treeFracSecEver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c3PftFrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c4PftFrac</t>
-  </si>
-  <si>
     <t xml:space="preserve">rGrowth</t>
   </si>
   <si>
@@ -824,15 +830,6 @@
   </si>
   <si>
     <t xml:space="preserve">Can not be produced by LPJ-GUESS: Same as r*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nppLeaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nppWood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nppRoot</t>
   </si>
   <si>
     <t xml:space="preserve">Not available inLPJ-GUESS. Not available in PISCES, which means not available in NEMO.</t>
@@ -925,12 +922,14 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1017,10 +1016,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H226"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F226" activeCellId="0" sqref="F226"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A158" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A178" activeCellId="0" sqref="178:178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1096,7 +1095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -1983,30 +1982,30 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="0" t="s">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F57" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="G56" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="0" t="s">
+      <c r="G57" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="F58" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G58" s="0" t="s">
+      <c r="G59" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F60" s="0" t="s">
         <v>123</v>
       </c>
       <c r="G60" s="0" t="s">
@@ -2018,7 +2017,7 @@
         <v>124</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>112</v>
@@ -2026,10 +2025,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F62" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="G62" s="0" t="s">
         <v>112</v>
@@ -2040,7 +2039,7 @@
         <v>127</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G63" s="0" t="s">
         <v>112</v>
@@ -2048,10 +2047,10 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G64" s="0" t="s">
         <v>112</v>
@@ -2059,10 +2058,10 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>112</v>
@@ -2070,10 +2069,10 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>112</v>
@@ -2081,10 +2080,10 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>112</v>
@@ -2092,10 +2091,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>112</v>
@@ -2103,10 +2102,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>112</v>
@@ -2114,10 +2113,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>112</v>
@@ -2125,10 +2124,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>112</v>
@@ -2136,10 +2135,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>112</v>
@@ -2147,10 +2146,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G73" s="0" t="s">
         <v>112</v>
@@ -2158,10 +2157,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="G74" s="0" t="s">
         <v>112</v>
@@ -2205,7 +2204,7 @@
         <v>145</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G78" s="0" t="s">
         <v>112</v>
@@ -2213,10 +2212,10 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G79" s="0" t="s">
         <v>112</v>
@@ -2224,10 +2223,10 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G80" s="0" t="s">
         <v>112</v>
@@ -2235,10 +2234,10 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G81" s="0" t="s">
         <v>112</v>
@@ -2246,10 +2245,10 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G82" s="0" t="s">
         <v>112</v>
@@ -2257,10 +2256,10 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G83" s="0" t="s">
         <v>112</v>
@@ -2268,10 +2267,10 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G84" s="0" t="s">
         <v>112</v>
@@ -2279,10 +2278,10 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G85" s="0" t="s">
         <v>112</v>
@@ -2290,10 +2289,10 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="G86" s="0" t="s">
         <v>112</v>
@@ -2301,10 +2300,10 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F87" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="G87" s="0" t="s">
         <v>112</v>
@@ -2315,7 +2314,7 @@
         <v>156</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G88" s="0" t="s">
         <v>112</v>
@@ -2323,10 +2322,10 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G89" s="0" t="s">
         <v>112</v>
@@ -2334,10 +2333,10 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G90" s="0" t="s">
         <v>112</v>
@@ -2345,10 +2344,10 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G91" s="0" t="s">
         <v>112</v>
@@ -2356,10 +2355,10 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G92" s="0" t="s">
         <v>112</v>
@@ -2367,10 +2366,10 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F93" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="F93" s="0" t="s">
-        <v>157</v>
       </c>
       <c r="G93" s="0" t="s">
         <v>112</v>
@@ -2381,7 +2380,7 @@
         <v>163</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G94" s="0" t="s">
         <v>112</v>
@@ -2389,10 +2388,10 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="F95" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="F95" s="0" t="s">
-        <v>164</v>
       </c>
       <c r="G95" s="0" t="s">
         <v>112</v>
@@ -2403,7 +2402,7 @@
         <v>166</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G96" s="0" t="s">
         <v>112</v>
@@ -2411,10 +2410,10 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G97" s="0" t="s">
         <v>112</v>
@@ -2422,10 +2421,10 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F98" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="F98" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="G98" s="0" t="s">
         <v>112</v>
@@ -2436,7 +2435,7 @@
         <v>170</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G99" s="0" t="s">
         <v>112</v>
@@ -2444,10 +2443,10 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G100" s="0" t="s">
         <v>112</v>
@@ -2455,10 +2454,10 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F101" s="0" t="s">
         <v>173</v>
-      </c>
-      <c r="F101" s="0" t="s">
-        <v>171</v>
       </c>
       <c r="G101" s="0" t="s">
         <v>112</v>
@@ -2469,7 +2468,7 @@
         <v>174</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G102" s="0" t="s">
         <v>112</v>
@@ -2477,10 +2476,10 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="F103" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="F103" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="G103" s="0" t="s">
         <v>112</v>
@@ -2491,7 +2490,7 @@
         <v>177</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G104" s="0" t="s">
         <v>112</v>
@@ -2499,10 +2498,10 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="F105" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="F105" s="0" t="s">
-        <v>175</v>
       </c>
       <c r="G105" s="0" t="s">
         <v>112</v>
@@ -2513,7 +2512,7 @@
         <v>180</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G106" s="0" t="s">
         <v>112</v>
@@ -2521,10 +2520,10 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G107" s="0" t="s">
         <v>112</v>
@@ -2532,10 +2531,10 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G108" s="0" t="s">
         <v>112</v>
@@ -2543,10 +2542,10 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F109" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="F109" s="0" t="s">
-        <v>181</v>
       </c>
       <c r="G109" s="0" t="s">
         <v>112</v>
@@ -2557,7 +2556,7 @@
         <v>185</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G110" s="0" t="s">
         <v>112</v>
@@ -2565,10 +2564,10 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G111" s="0" t="s">
         <v>112</v>
@@ -2576,10 +2575,10 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G112" s="0" t="s">
         <v>112</v>
@@ -2587,10 +2586,10 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G113" s="0" t="s">
         <v>112</v>
@@ -2598,10 +2597,10 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F114" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G114" s="0" t="s">
         <v>112</v>
@@ -2609,10 +2608,10 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G115" s="0" t="s">
         <v>112</v>
@@ -2620,10 +2619,10 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F116" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G116" s="0" t="s">
         <v>112</v>
@@ -2631,10 +2630,10 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G117" s="0" t="s">
         <v>112</v>
@@ -2642,10 +2641,10 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F118" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G118" s="0" t="s">
         <v>112</v>
@@ -2653,10 +2652,10 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G119" s="0" t="s">
         <v>112</v>
@@ -2664,10 +2663,10 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="0" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F120" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G120" s="0" t="s">
         <v>112</v>
@@ -2675,10 +2674,10 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F121" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G121" s="0" t="s">
         <v>112</v>
@@ -2686,10 +2685,10 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F122" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G122" s="0" t="s">
         <v>112</v>
@@ -2697,10 +2696,10 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F123" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G123" s="0" t="s">
         <v>112</v>
@@ -2708,10 +2707,10 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F124" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G124" s="0" t="s">
         <v>112</v>
@@ -2719,10 +2718,10 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G125" s="0" t="s">
         <v>112</v>
@@ -2730,10 +2729,10 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F126" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G126" s="0" t="s">
         <v>112</v>
@@ -2741,10 +2740,10 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G127" s="0" t="s">
         <v>112</v>
@@ -2752,10 +2751,10 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F128" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G128" s="0" t="s">
         <v>112</v>
@@ -2763,10 +2762,10 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G129" s="0" t="s">
         <v>112</v>
@@ -2774,10 +2773,10 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F130" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G130" s="0" t="s">
         <v>112</v>
@@ -2785,10 +2784,10 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F131" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G131" s="0" t="s">
         <v>112</v>
@@ -2796,10 +2795,10 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F132" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G132" s="0" t="s">
         <v>112</v>
@@ -2807,10 +2806,10 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F133" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G133" s="0" t="s">
         <v>112</v>
@@ -2818,10 +2817,10 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F134" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G134" s="0" t="s">
         <v>112</v>
@@ -2829,10 +2828,10 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F135" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G135" s="0" t="s">
         <v>112</v>
@@ -2840,10 +2839,10 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F136" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G136" s="0" t="s">
         <v>112</v>
@@ -2851,10 +2850,10 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F137" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G137" s="0" t="s">
         <v>112</v>
@@ -2862,10 +2861,10 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F138" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G138" s="0" t="s">
         <v>112</v>
@@ -2873,10 +2872,10 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F139" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="F139" s="0" t="s">
-        <v>186</v>
       </c>
       <c r="G139" s="0" t="s">
         <v>112</v>
@@ -2901,29 +2900,29 @@
         <v>219</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F142" s="0" t="s">
         <v>219</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G143" s="0" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2931,106 +2930,106 @@
         <v>223</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="0" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F145" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F146" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G146" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="0" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F147" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G147" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F148" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F149" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G149" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
-        <v>231</v>
+        <v>119</v>
       </c>
       <c r="F150" s="0" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="G150" s="0" t="s">
-        <v>225</v>
+        <v>112</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="0" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F151" s="0" t="s">
-        <v>224</v>
+        <v>179</v>
       </c>
       <c r="G151" s="0" t="s">
-        <v>225</v>
+        <v>112</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F152" s="0" t="s">
-        <v>224</v>
+        <v>126</v>
       </c>
       <c r="G152" s="0" t="s">
-        <v>225</v>
+        <v>112</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="0" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="F153" s="0" t="s">
-        <v>234</v>
+        <v>126</v>
       </c>
       <c r="G153" s="0" t="s">
         <v>112</v>
@@ -3038,10 +3037,10 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="0" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
       <c r="F154" s="0" t="s">
-        <v>235</v>
+        <v>126</v>
       </c>
       <c r="G154" s="0" t="s">
         <v>112</v>
@@ -3049,10 +3048,10 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="0" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F155" s="0" t="s">
-        <v>181</v>
+        <v>126</v>
       </c>
       <c r="G155" s="0" t="s">
         <v>112</v>
@@ -3060,10 +3059,10 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="0" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F156" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G156" s="0" t="s">
         <v>112</v>
@@ -3071,10 +3070,10 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="0" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F157" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G157" s="0" t="s">
         <v>112</v>
@@ -3082,10 +3081,10 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="0" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F158" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G158" s="0" t="s">
         <v>112</v>
@@ -3093,10 +3092,10 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="0" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F159" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G159" s="0" t="s">
         <v>112</v>
@@ -3104,64 +3103,64 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="0" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F160" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G160" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="F161" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G161" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="F162" s="0" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="G162" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="F163" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G163" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="0" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F164" s="0" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G164" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C165" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F165" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G165" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="F166" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="G166" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="G166" s="0" t="s">
+      <c r="F167" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="G167" s="0" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3170,7 +3169,7 @@
         <v>247</v>
       </c>
       <c r="F168" s="0" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="G168" s="0" t="s">
         <v>112</v>
@@ -3181,7 +3180,7 @@
         <v>248</v>
       </c>
       <c r="F169" s="0" t="s">
-        <v>249</v>
+        <v>155</v>
       </c>
       <c r="G169" s="0" t="s">
         <v>112</v>
@@ -3189,10 +3188,10 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F170" s="0" t="s">
-        <v>251</v>
+        <v>155</v>
       </c>
       <c r="G170" s="0" t="s">
         <v>112</v>
@@ -3200,10 +3199,10 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="0" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F171" s="0" t="s">
-        <v>253</v>
+        <v>155</v>
       </c>
       <c r="G171" s="0" t="s">
         <v>112</v>
@@ -3211,10 +3210,10 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="0" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F172" s="0" t="s">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="G172" s="0" t="s">
         <v>112</v>
@@ -3222,10 +3221,10 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F173" s="0" t="s">
-        <v>257</v>
+        <v>155</v>
       </c>
       <c r="G173" s="0" t="s">
         <v>112</v>
@@ -3233,10 +3232,10 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="0" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F174" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G174" s="0" t="s">
         <v>112</v>
@@ -3244,32 +3243,21 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="0" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F175" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G175" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="F176" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="G176" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="0" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F177" s="0" t="s">
-        <v>157</v>
+        <v>256</v>
       </c>
       <c r="G177" s="0" t="s">
         <v>112</v>
@@ -3277,10 +3265,10 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C178" s="0" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F178" s="0" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="G178" s="0" t="s">
         <v>112</v>
@@ -3288,10 +3276,10 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="0" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F179" s="0" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="G179" s="0" t="s">
         <v>112</v>
@@ -3299,10 +3287,10 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="0" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F180" s="0" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G180" s="0" t="s">
         <v>112</v>
@@ -3310,10 +3298,10 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="0" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F181" s="0" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G181" s="0" t="s">
         <v>112</v>
@@ -3321,10 +3309,10 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="0" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F182" s="0" t="s">
-        <v>157</v>
+        <v>265</v>
       </c>
       <c r="G182" s="0" t="s">
         <v>112</v>
@@ -3332,10 +3320,10 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="0" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F183" s="0" t="s">
-        <v>157</v>
+        <v>267</v>
       </c>
       <c r="G183" s="0" t="s">
         <v>112</v>
@@ -3343,24 +3331,13 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="0" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F184" s="0" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
       <c r="G184" s="0" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="F186" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G186" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,260 +3345,265 @@
         <v>200</v>
       </c>
       <c r="F187" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G187" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G187" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C188" s="0" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F188" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G188" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G188" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F189" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G189" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G189" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="0" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F190" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G190" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G190" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C191" s="0" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F191" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G191" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G191" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C192" s="0" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F192" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G192" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G192" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F193" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G193" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="G193" s="0" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="F195" s="2" t="s">
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C194" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G194" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G195" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C196" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F196" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G196" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G196" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C197" s="0" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F197" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G197" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G197" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="0" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="F198" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G198" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G198" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C199" s="0" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F199" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G199" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="G199" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C200" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F200" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G200" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="G200" s="0" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F215" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="G215" s="5" t="s">
-        <v>275</v>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C201" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G201" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C216" s="0" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F216" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G216" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G216" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C217" s="0" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F217" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G217" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G217" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C218" s="0" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F218" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G218" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G218" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C219" s="0" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F219" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G219" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G219" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C220" s="0" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F220" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G220" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G220" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C221" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F221" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G221" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G221" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C222" s="0" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F222" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G222" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G222" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C223" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F223" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G223" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C224" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="F224" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G224" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C226" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F223" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="G223" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="2" t="s">
+      <c r="F226" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="F225" s="0" t="s">
+      <c r="G226" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="G225" s="0" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
NEMO related updates from shared google doc in pre ignored file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="326">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -878,6 +878,126 @@
   </si>
   <si>
     <t xml:space="preserve">Raffaele Bernardello, David Docquier, Thomas Reerink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volcello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid-cell volume ca. 2000.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftmz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA before CMIP6 starts. zomsflgo requires the subasins.nc file and a namelist parameter (Poleward Transport Diagnostic) / basin-wide variables are: zomsfatl zomsfpac zomsfind zomsfipc. NEMO-OPA - volume meridional stream function is available (zomsfglo). Maybe mass streamfunction can be obtained multiplying it by potential density (sea_water_sigma_theta) in the file_def xml ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etienne Tourigny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overturning mass streamfunction arising from all advective mass transport processes, resolved and parameterized.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftmrho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA before CMIP6 starts. NEMO-OPA - volume meridional stream function is available (zomsfglo). Maybe mass streamfunction can be obtained multiplying it by potential density (sea_water_sigma_theta) in the file_def xml ?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftyrho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA before CMIP6 starts. NEMO-OPA - I guess it's the same as above only rotated in case y does not align exactly with north-south direction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftmzmpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA before CMIP6 starts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMIP5 called this 'due to Bolus Advection'.  Name change respects the more general physics of the mesoscale parameterizations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftmrhompa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftyzmpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftyrhompa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftmzsmpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report only if there is a submesoscale eddy parameterization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msftyzsmpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfbasinpmdiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions to heat transport from parameterized mesoscale eddy-induced diffusive transport (i.e., neutral diffusion). Diagnosed here as a function of latitude and basin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfbasinpsmadv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions to heat transport from parameterized mesoscale eddy-induced advective transport. Diagnosed here as a function of latitude and basin.  Use Celsius for temperature scale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfbasinpadv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions to heat transport from parameterized eddy-induced advective transport due to any subgrid advective process. Diagnosed here as a function of latitude and basin.  Use Celsius for temperature scale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wfcorr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive flux implies correction adds water to ocean.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfriver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA, i.e. it makes no sence to make it availble because it is zero. It looks like it is assumed zero in NEMO, not 100% sure though.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field is physical, and it arises when rivers carry a nonzero salt content.  Often this is zero, with rivers assumed to be fresh.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfsifrazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-LIM, not in NEMO anywhere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfsifrazil2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfcorr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauucorr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the stress on the liquid ocean from overlying atmosphere, sea ice, ice shelf, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauvcorr</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1136,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H226"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A158" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A178" activeCellId="0" sqref="178:178"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A236" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A234" activeCellId="0" sqref="A234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3604,6 +3724,295 @@
         <v>285</v>
       </c>
     </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C233" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="F233" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G233" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I233" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C235" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="F235" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C236" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F236" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="G236" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="I236" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C237" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="F237" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="G237" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I237" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C238" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="F238" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="G238" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I238" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C239" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="F239" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G239" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I239" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C240" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="F240" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G240" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I240" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C241" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="F241" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G241" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I241" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C242" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="F242" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G242" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I242" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C243" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F243" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G243" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I243" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C244" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="F244" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G244" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I244" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C245" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="F245" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G245" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I245" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C246" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="F246" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G246" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I246" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C247" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F247" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="G247" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I247" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C248" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="F248" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G248" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I248" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C249" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="F249" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="G249" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I249" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C250" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="F250" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="G250" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C251" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="F251" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="G251" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C252" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="F252" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G252" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C253" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="F253" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G253" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I253" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C254" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="F254" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G254" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="I254" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Small comment adjustment in the pre ignored file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Air Pressure at Convective Cloud Base</t>
   </si>
   <si>
-    <t xml:space="preserve">Too much effort?: convective cloud cover ccc[185] &gt; 0.5 or &gt; 0.0, this mask combine with cloud base height cbh[228023], therafter with surface pressure sp[134] and lapse rate the cct can be calculated</t>
+    <t xml:space="preserve">Too much effort?: convective cloud cover ccc[128185 i.e in table 128] &gt; 0.5 or &gt; 0.0, this mask combine with cloud base height cbh[228023], therafter with surface pressure sp[134] and lapse rate the cct can be calculated</t>
   </si>
   <si>
     <t xml:space="preserve">Where convective cloud is present in the grid cell, the instantaneous cloud base altitude should be that of the bottom of the lowest level containing convective cloud. Missing data should be reported in the absence of convective cloud. The time mean should be calculated from these quantities averaging over occasions when convective cloud is present only, and should contain missing data for occasions when no convective cloud is present during the meaning period.</t>
@@ -1129,8 +1129,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A231" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A248" activeCellId="0" sqref="A248"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Address #298 removing the miss identified TM5 variables from the tm5par.json and adding them to the pre-ignored list.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="567">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -755,6 +755,45 @@
   </si>
   <si>
     <t xml:space="preserve">longitude latitude alevel time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nh50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommi Bergman, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550csaer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in TM5. For h2o, TM5 cannot do all phases of water, should therefore come from IFS if anywhere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in TM5. CO2 only transported in C-Cycle version, unclear if it is needed as output from TM5?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2massclim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2antt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2fos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2nat</t>
   </si>
   <si>
     <t xml:space="preserve">Snow Age</t>
@@ -1710,7 +1749,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1740,13 +1779,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1838,16 +1870,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1863,23 +1891,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1900,10 +1928,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K466"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A416" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D444" activeCellId="0" sqref="D444"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A174" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B182" activeCellId="0" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1952,7 +1980,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1998,27 +2026,27 @@
       <c r="E4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2369,9 +2397,9 @@
       <c r="B37" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
       <c r="H37" s="0" t="s">
         <v>53</v>
       </c>
@@ -2386,9 +2414,9 @@
       <c r="B38" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
       <c r="H38" s="0" t="s">
         <v>53</v>
       </c>
@@ -2400,23 +2428,23 @@
       <c r="A39" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5" t="s">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4" t="s">
         <v>69</v>
       </c>
       <c r="I40" s="0" t="s">
@@ -2424,15 +2452,15 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4" t="s">
         <v>69</v>
       </c>
       <c r="I41" s="0" t="s">
@@ -2443,15 +2471,15 @@
       <c r="A42" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5" t="s">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4" t="s">
         <v>69</v>
       </c>
       <c r="I42" s="0" t="s">
@@ -2462,15 +2490,15 @@
       <c r="A43" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5" t="s">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4" t="s">
         <v>69</v>
       </c>
       <c r="I43" s="0" t="s">
@@ -2481,27 +2509,27 @@
       <c r="A44" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4" t="s">
         <v>75</v>
       </c>
       <c r="I45" s="0" t="s">
@@ -2512,12 +2540,12 @@
       <c r="A46" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="H46" s="5" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="H46" s="4" t="s">
         <v>75</v>
       </c>
       <c r="I46" s="0" t="s">
@@ -2528,12 +2556,12 @@
       <c r="A47" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="H47" s="5" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="H47" s="4" t="s">
         <v>75</v>
       </c>
       <c r="I47" s="0" t="s">
@@ -2544,12 +2572,12 @@
       <c r="A48" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="H48" s="5" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="H48" s="4" t="s">
         <v>75</v>
       </c>
       <c r="I48" s="0" t="s">
@@ -4290,140 +4318,143 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D182" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E182" s="0" t="s">
+      <c r="B182" s="0" t="s">
         <v>245</v>
+      </c>
+      <c r="H182" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="I182" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="H183" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="I183" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="H184" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="I184" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="H184" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="I184" s="0" t="s">
-        <v>248</v>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B185" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="H185" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="I185" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B186" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="H186" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="I186" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B187" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="H187" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="I187" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="H188" s="0" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="I188" s="0" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H189" s="0" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="I189" s="0" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H190" s="0" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="I190" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B192" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="H192" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="I192" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B191" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="H194" s="0" t="s">
+      <c r="H191" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="I191" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D195" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" s="0" t="s">
         <v>258</v>
-      </c>
-      <c r="I194" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B196" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="I196" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H197" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="H197" s="0" t="s">
+      <c r="I197" s="0" t="s">
         <v>261</v>
-      </c>
-      <c r="I197" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="H198" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="I198" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B199" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="H199" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I199" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H200" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I200" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H201" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I201" s="0" t="s">
         <v>170</v>
@@ -4431,10 +4462,10 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="0" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H202" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I202" s="0" t="s">
         <v>170</v>
@@ -4442,76 +4473,40 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="0" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H203" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="I203" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="H204" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I204" s="0" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="0" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H205" s="0" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="I205" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B206" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="H206" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I206" s="0" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H207" s="0" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="I207" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B208" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="H208" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I208" s="0" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="H209" s="0" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="I209" s="0" t="s">
         <v>170</v>
@@ -4519,10 +4514,10 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="0" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="H210" s="0" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="I210" s="0" t="s">
         <v>170</v>
@@ -4533,7 +4528,7 @@
         <v>275</v>
       </c>
       <c r="H211" s="0" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I211" s="0" t="s">
         <v>170</v>
@@ -4541,10 +4536,10 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="H212" s="0" t="s">
         <v>277</v>
-      </c>
-      <c r="H212" s="0" t="s">
-        <v>278</v>
       </c>
       <c r="I212" s="0" t="s">
         <v>170</v>
@@ -4552,10 +4547,10 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H213" s="0" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I213" s="0" t="s">
         <v>170</v>
@@ -4563,10 +4558,10 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H214" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I214" s="0" t="s">
         <v>170</v>
@@ -4574,10 +4569,10 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H215" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I215" s="0" t="s">
         <v>170</v>
@@ -4585,10 +4580,10 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H216" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I216" s="0" t="s">
         <v>170</v>
@@ -4596,10 +4591,10 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="0" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H217" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I217" s="0" t="s">
         <v>170</v>
@@ -4607,10 +4602,10 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="0" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H218" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I218" s="0" t="s">
         <v>170</v>
@@ -4618,10 +4613,10 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H219" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I219" s="0" t="s">
         <v>170</v>
@@ -4629,10 +4624,10 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H220" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I220" s="0" t="s">
         <v>170</v>
@@ -4640,10 +4635,10 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="0" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I221" s="0" t="s">
         <v>170</v>
@@ -4651,10 +4646,10 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="I222" s="0" t="s">
         <v>170</v>
@@ -4662,10 +4657,10 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="H223" s="0" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="I223" s="0" t="s">
         <v>170</v>
@@ -4673,10 +4668,10 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H224" s="0" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I224" s="0" t="s">
         <v>170</v>
@@ -4684,10 +4679,10 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H225" s="0" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I225" s="0" t="s">
         <v>170</v>
@@ -4695,7 +4690,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H226" s="0" t="s">
         <v>293</v>
@@ -4706,10 +4701,10 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H227" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="I227" s="0" t="s">
         <v>170</v>
@@ -4717,10 +4712,10 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H228" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="I228" s="0" t="s">
         <v>170</v>
@@ -4728,10 +4723,10 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H229" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="I229" s="0" t="s">
         <v>170</v>
@@ -4739,10 +4734,10 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H230" s="0" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I230" s="0" t="s">
         <v>170</v>
@@ -4750,10 +4745,10 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H231" s="0" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I231" s="0" t="s">
         <v>170</v>
@@ -4761,10 +4756,10 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H232" s="0" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I232" s="0" t="s">
         <v>170</v>
@@ -4772,10 +4767,10 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H233" s="0" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I233" s="0" t="s">
         <v>170</v>
@@ -4783,10 +4778,10 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H234" s="0" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I234" s="0" t="s">
         <v>170</v>
@@ -4794,10 +4789,10 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H235" s="0" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="I235" s="0" t="s">
         <v>170</v>
@@ -4805,10 +4800,10 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H236" s="0" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="I236" s="0" t="s">
         <v>170</v>
@@ -4816,10 +4811,10 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="H237" s="0" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I237" s="0" t="s">
         <v>170</v>
@@ -4827,10 +4822,10 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H238" s="0" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I238" s="0" t="s">
         <v>170</v>
@@ -4838,10 +4833,10 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H239" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="I239" s="0" t="s">
         <v>170</v>
@@ -4849,10 +4844,10 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="0" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H240" s="0" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I240" s="0" t="s">
         <v>170</v>
@@ -4860,10 +4855,10 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="0" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H241" s="0" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I241" s="0" t="s">
         <v>170</v>
@@ -4871,10 +4866,10 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="0" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H242" s="0" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="I242" s="0" t="s">
         <v>170</v>
@@ -4882,10 +4877,10 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="0" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="H243" s="0" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I243" s="0" t="s">
         <v>170</v>
@@ -4893,10 +4888,10 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="0" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="H244" s="0" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I244" s="0" t="s">
         <v>170</v>
@@ -4904,10 +4899,10 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="H245" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I245" s="0" t="s">
         <v>170</v>
@@ -4915,10 +4910,10 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="0" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H246" s="0" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I246" s="0" t="s">
         <v>170</v>
@@ -4926,10 +4921,10 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="0" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="H247" s="0" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I247" s="0" t="s">
         <v>170</v>
@@ -4937,10 +4932,10 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="0" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="H248" s="0" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I248" s="0" t="s">
         <v>170</v>
@@ -4948,10 +4943,10 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="0" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="H249" s="0" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I249" s="0" t="s">
         <v>170</v>
@@ -4959,10 +4954,10 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="0" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H250" s="0" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I250" s="0" t="s">
         <v>170</v>
@@ -4970,10 +4965,10 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="0" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H251" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="I251" s="0" t="s">
         <v>170</v>
@@ -4981,10 +4976,10 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="0" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H252" s="0" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I252" s="0" t="s">
         <v>170</v>
@@ -4992,10 +4987,10 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="0" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H253" s="0" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="I253" s="0" t="s">
         <v>170</v>
@@ -5003,10 +4998,10 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="0" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H254" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="I254" s="0" t="s">
         <v>170</v>
@@ -5014,10 +5009,10 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="0" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H255" s="0" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="I255" s="0" t="s">
         <v>170</v>
@@ -5025,10 +5020,10 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H256" s="0" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="I256" s="0" t="s">
         <v>170</v>
@@ -5036,10 +5031,10 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="0" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H257" s="0" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="I257" s="0" t="s">
         <v>170</v>
@@ -5047,10 +5042,10 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H258" s="0" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="I258" s="0" t="s">
         <v>170</v>
@@ -5058,10 +5053,10 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="H259" s="0" t="s">
         <v>335</v>
-      </c>
-      <c r="H259" s="0" t="s">
-        <v>322</v>
       </c>
       <c r="I259" s="0" t="s">
         <v>170</v>
@@ -5072,7 +5067,7 @@
         <v>336</v>
       </c>
       <c r="H260" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I260" s="0" t="s">
         <v>170</v>
@@ -5083,7 +5078,7 @@
         <v>337</v>
       </c>
       <c r="H261" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I261" s="0" t="s">
         <v>170</v>
@@ -5094,7 +5089,7 @@
         <v>338</v>
       </c>
       <c r="H262" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I262" s="0" t="s">
         <v>170</v>
@@ -5105,7 +5100,7 @@
         <v>339</v>
       </c>
       <c r="H263" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I263" s="0" t="s">
         <v>170</v>
@@ -5116,7 +5111,7 @@
         <v>340</v>
       </c>
       <c r="H264" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I264" s="0" t="s">
         <v>170</v>
@@ -5127,7 +5122,7 @@
         <v>341</v>
       </c>
       <c r="H265" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I265" s="0" t="s">
         <v>170</v>
@@ -5138,7 +5133,7 @@
         <v>342</v>
       </c>
       <c r="H266" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I266" s="0" t="s">
         <v>170</v>
@@ -5149,7 +5144,7 @@
         <v>343</v>
       </c>
       <c r="H267" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I267" s="0" t="s">
         <v>170</v>
@@ -5160,7 +5155,7 @@
         <v>344</v>
       </c>
       <c r="H268" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I268" s="0" t="s">
         <v>170</v>
@@ -5171,7 +5166,7 @@
         <v>345</v>
       </c>
       <c r="H269" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I269" s="0" t="s">
         <v>170</v>
@@ -5182,7 +5177,7 @@
         <v>346</v>
       </c>
       <c r="H270" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I270" s="0" t="s">
         <v>170</v>
@@ -5193,7 +5188,7 @@
         <v>347</v>
       </c>
       <c r="H271" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I271" s="0" t="s">
         <v>170</v>
@@ -5204,7 +5199,7 @@
         <v>348</v>
       </c>
       <c r="H272" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I272" s="0" t="s">
         <v>170</v>
@@ -5215,7 +5210,7 @@
         <v>349</v>
       </c>
       <c r="H273" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I273" s="0" t="s">
         <v>170</v>
@@ -5226,7 +5221,7 @@
         <v>350</v>
       </c>
       <c r="H274" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I274" s="0" t="s">
         <v>170</v>
@@ -5237,7 +5232,7 @@
         <v>351</v>
       </c>
       <c r="H275" s="0" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="I275" s="0" t="s">
         <v>170</v>
@@ -5248,7 +5243,7 @@
         <v>352</v>
       </c>
       <c r="H276" s="0" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="I276" s="0" t="s">
         <v>170</v>
@@ -5256,10 +5251,10 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H277" s="0" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="I277" s="0" t="s">
         <v>170</v>
@@ -5267,109 +5262,109 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H278" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I278" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H279" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I279" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H280" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I280" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H281" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I281" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H282" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I282" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H283" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I283" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H284" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I284" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H285" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I285" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H286" s="0" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="I286" s="0" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="s">
-        <v>257</v>
+        <v>363</v>
       </c>
       <c r="H287" s="0" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="I287" s="0" t="s">
         <v>170</v>
@@ -5377,10 +5372,10 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="H288" s="0" t="s">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="I288" s="0" t="s">
         <v>170</v>
@@ -5388,10 +5383,10 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="H289" s="0" t="s">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="I289" s="0" t="s">
         <v>170</v>
@@ -5399,10 +5394,10 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H290" s="0" t="s">
-        <v>264</v>
+        <v>368</v>
       </c>
       <c r="I290" s="0" t="s">
         <v>170</v>
@@ -5410,13 +5405,13 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="H291" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="I291" s="0" t="s">
         <v>371</v>
-      </c>
-      <c r="H291" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I291" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5424,10 +5419,10 @@
         <v>372</v>
       </c>
       <c r="H292" s="0" t="s">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="I292" s="0" t="s">
-        <v>170</v>
+        <v>371</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5435,10 +5430,10 @@
         <v>373</v>
       </c>
       <c r="H293" s="0" t="s">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="I293" s="0" t="s">
-        <v>170</v>
+        <v>371</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5446,10 +5441,10 @@
         <v>374</v>
       </c>
       <c r="H294" s="0" t="s">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="I294" s="0" t="s">
-        <v>170</v>
+        <v>371</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5457,10 +5452,10 @@
         <v>375</v>
       </c>
       <c r="H295" s="0" t="s">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="I295" s="0" t="s">
-        <v>170</v>
+        <v>371</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5468,10 +5463,10 @@
         <v>376</v>
       </c>
       <c r="H296" s="0" t="s">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="I296" s="0" t="s">
-        <v>170</v>
+        <v>371</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5479,26 +5474,51 @@
         <v>377</v>
       </c>
       <c r="H297" s="0" t="s">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="I297" s="0" t="s">
-        <v>170</v>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B298" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="H298" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="I298" s="0" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
+      </c>
+      <c r="H299" s="0" t="s">
+        <v>370</v>
       </c>
       <c r="I299" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B300" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="H300" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="I300" s="0" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H301" s="0" t="s">
-        <v>256</v>
+        <v>330</v>
       </c>
       <c r="I301" s="0" t="s">
         <v>170</v>
@@ -5506,10 +5526,10 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="H302" s="0" t="s">
-        <v>381</v>
+        <v>277</v>
       </c>
       <c r="I302" s="0" t="s">
         <v>170</v>
@@ -5517,10 +5537,10 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H303" s="0" t="s">
-        <v>383</v>
+        <v>277</v>
       </c>
       <c r="I303" s="0" t="s">
         <v>170</v>
@@ -5531,7 +5551,7 @@
         <v>384</v>
       </c>
       <c r="H304" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I304" s="0" t="s">
         <v>170</v>
@@ -5542,7 +5562,7 @@
         <v>385</v>
       </c>
       <c r="H305" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I305" s="0" t="s">
         <v>170</v>
@@ -5553,7 +5573,7 @@
         <v>386</v>
       </c>
       <c r="H306" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I306" s="0" t="s">
         <v>170</v>
@@ -5564,7 +5584,7 @@
         <v>387</v>
       </c>
       <c r="H307" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I307" s="0" t="s">
         <v>170</v>
@@ -5575,7 +5595,7 @@
         <v>388</v>
       </c>
       <c r="H308" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I308" s="0" t="s">
         <v>170</v>
@@ -5586,7 +5606,7 @@
         <v>389</v>
       </c>
       <c r="H309" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I309" s="0" t="s">
         <v>170</v>
@@ -5597,29 +5617,15 @@
         <v>390</v>
       </c>
       <c r="H310" s="0" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="I310" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B311" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="H311" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="I311" s="0" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="H312" s="0" t="s">
-        <v>293</v>
+        <v>391</v>
       </c>
       <c r="I312" s="0" t="s">
         <v>170</v>
@@ -5627,408 +5633,466 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="H314" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
+      </c>
+      <c r="H314" s="0" t="s">
+        <v>269</v>
       </c>
       <c r="I314" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="H315" s="3" t="s">
         <v>393</v>
       </c>
+      <c r="H315" s="0" t="s">
+        <v>394</v>
+      </c>
       <c r="I315" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B316" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="H316" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
+      </c>
+      <c r="H316" s="0" t="s">
+        <v>396</v>
       </c>
       <c r="I316" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="H317" s="3" t="s">
-        <v>393</v>
+        <v>397</v>
+      </c>
+      <c r="H317" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I317" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="H318" s="3" t="s">
-        <v>393</v>
+        <v>398</v>
+      </c>
+      <c r="H318" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I318" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B319" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="H319" s="3" t="s">
-        <v>393</v>
+        <v>399</v>
+      </c>
+      <c r="H319" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I319" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="H320" s="3" t="s">
-        <v>393</v>
+        <v>400</v>
+      </c>
+      <c r="H320" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I320" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="H321" s="3" t="s">
-        <v>393</v>
+        <v>401</v>
+      </c>
+      <c r="H321" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I321" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B322" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="H322" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="I322" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="H323" s="3" t="s">
-        <v>393</v>
+        <v>403</v>
+      </c>
+      <c r="H323" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I323" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="H324" s="3" t="s">
-        <v>393</v>
+        <v>404</v>
+      </c>
+      <c r="H324" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I324" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="H325" s="3" t="s">
-        <v>393</v>
+        <v>405</v>
+      </c>
+      <c r="H325" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="I325" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B326" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="H326" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="I326" s="0" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="H327" s="3" t="s">
-        <v>393</v>
+        <v>351</v>
+      </c>
+      <c r="H327" s="2" t="s">
+        <v>406</v>
       </c>
       <c r="I327" s="0" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="H328" s="3" t="s">
-        <v>393</v>
+        <v>349</v>
+      </c>
+      <c r="H328" s="2" t="s">
+        <v>406</v>
       </c>
       <c r="I328" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B343" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="H343" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I343" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B344" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="H344" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I344" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B345" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="H345" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I345" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B346" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="H346" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I346" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B347" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="H347" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I347" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B348" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="H348" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I348" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B349" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="H349" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I349" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B350" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="H350" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I350" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B351" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="H351" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="I351" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B329" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="H329" s="2" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="0" t="s">
+      <c r="I329" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B330" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="H330" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B353" s="3" t="s">
+      <c r="I330" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="C353" s="3"/>
-      <c r="D353" s="3"/>
-      <c r="H353" s="0" t="s">
+    </row>
+    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B331" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="H331" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I331" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B332" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="H332" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I332" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B333" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="H333" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I333" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B334" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="H334" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I334" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B336" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="H336" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I336" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B337" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="H337" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I337" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B338" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="H338" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I338" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B339" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="H339" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I339" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B340" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="H340" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I340" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B341" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="H341" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I341" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B356" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="I353" s="0" t="s">
+      <c r="H356" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="0" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="B355" s="0" t="s">
+      <c r="I356" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="H355" s="0" t="s">
+    </row>
+    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B357" s="0" t="s">
         <v>411</v>
       </c>
-      <c r="I355" s="0" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="B356" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="H356" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="I356" s="0" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="B357" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="H357" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="I357" s="0" t="s">
-        <v>412</v>
+      <c r="H357" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I357" s="6" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B358" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="H358" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="I358" s="0" t="s">
         <v>412</v>
+      </c>
+      <c r="H358" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I358" s="6" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="H359" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="I359" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
+      </c>
+      <c r="H359" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I359" s="6" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B360" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="H360" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I360" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B361" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="H361" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I361" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B362" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="H362" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I362" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B363" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="H363" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I363" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B364" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="H360" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="I360" s="0" t="s">
-        <v>412</v>
+      <c r="H364" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I364" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B366" s="0" t="s">
+      <c r="A366" s="0" t="s">
         <v>419</v>
       </c>
+      <c r="B366" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C366" s="2"/>
+      <c r="D366" s="2"/>
       <c r="H366" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I366" s="0" t="s">
-        <v>397</v>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>419</v>
+      </c>
       <c r="B368" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="H368" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
+      </c>
+      <c r="I368" s="0" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>419</v>
+      </c>
       <c r="B369" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="H369" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="I369" s="0" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>419</v>
+      </c>
       <c r="B370" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H370" s="0" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I370" s="0" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H371" s="0" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="I371" s="0" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6036,605 +6100,536 @@
         <v>430</v>
       </c>
       <c r="H372" s="0" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="I372" s="0" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H373" s="0" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="I373" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B374" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="H374" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="I374" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B375" s="0" t="s">
-        <v>434</v>
-      </c>
-      <c r="H375" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="I375" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B376" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="H376" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="I376" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B377" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="H377" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="I377" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B378" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="H378" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="I378" s="0" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B379" s="0" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="H379" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="I379" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B380" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="H380" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="I380" s="0" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="0" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="H381" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="I381" s="0" t="s">
-        <v>397</v>
+        <v>435</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="0" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H382" s="0" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="I382" s="0" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="H383" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="I383" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B384" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="H384" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="I384" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B385" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="H385" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="H383" s="0" t="s">
-        <v>443</v>
-      </c>
-      <c r="I383" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="0" t="s">
+      <c r="I385" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B386" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="B384" s="0" t="s">
+      <c r="H386" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I386" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B387" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="H384" s="0" t="s">
-        <v>420</v>
-      </c>
-      <c r="I384" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B385" s="0" t="s">
+      <c r="H387" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I387" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B388" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="H385" s="0" t="s">
-        <v>420</v>
-      </c>
-      <c r="I385" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="0" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B387" s="0" t="s">
+      <c r="H388" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I388" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B389" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="H387" s="0" t="s">
+      <c r="H389" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I389" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B390" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="I387" s="0" t="s">
+      <c r="H390" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I390" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B391" s="0" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B388" s="0" t="s">
+      <c r="H391" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I391" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B392" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="H388" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I388" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B389" s="0" t="s">
+      <c r="H392" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I392" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B393" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="H389" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I389" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B390" s="0" t="s">
+      <c r="H393" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="I393" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B394" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="H390" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I390" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B391" s="0" t="s">
+      <c r="H394" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="H391" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I391" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B392" s="0" t="s">
+      <c r="I394" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B395" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="H392" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I392" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B393" s="0" t="s">
+      <c r="H395" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="H393" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I393" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B394" s="0" t="s">
+      <c r="I395" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B396" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="H394" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I394" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B395" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="H395" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I395" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B396" s="0" t="s">
-        <v>459</v>
-      </c>
       <c r="H396" s="0" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="I396" s="0" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="B397" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H397" s="0" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="I397" s="0" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="B398" s="0" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H398" s="0" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="I398" s="0" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B399" s="0" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B400" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="H400" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="H399" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I399" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B400" s="0" t="s">
+      <c r="I400" s="0" t="s">
         <v>463</v>
-      </c>
-      <c r="H400" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="I400" s="0" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B401" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="B401" s="0" t="s">
-        <v>465</v>
-      </c>
       <c r="H401" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I401" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B402" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H402" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I402" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>464</v>
+        <v>458</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="H403" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="I403" s="0" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B404" s="0" t="s">
         <v>467</v>
       </c>
       <c r="H404" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I404" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B405" s="0" t="s">
         <v>468</v>
       </c>
       <c r="H405" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I405" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="0" t="s">
+        <v>458</v>
+      </c>
       <c r="B406" s="0" t="s">
         <v>469</v>
       </c>
       <c r="H406" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I406" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="0" t="s">
+        <v>458</v>
+      </c>
       <c r="B407" s="0" t="s">
         <v>470</v>
       </c>
       <c r="H407" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I407" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="0" t="s">
+        <v>458</v>
+      </c>
       <c r="B408" s="0" t="s">
         <v>471</v>
       </c>
       <c r="H408" s="0" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="I408" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="412" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B409" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="H409" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="I409" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B410" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="H410" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="I410" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B411" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="H411" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="I411" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="0" t="s">
+        <v>458</v>
+      </c>
       <c r="B412" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="H412" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I412" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="413" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B413" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="H413" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I413" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="414" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="0" t="s">
+        <v>477</v>
+      </c>
       <c r="B414" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="H414" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I414" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="0" t="s">
+        <v>477</v>
+      </c>
       <c r="B415" s="0" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="H415" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I415" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="416" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B416" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="H416" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="I416" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="417" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="0" t="s">
+        <v>477</v>
+      </c>
       <c r="B417" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="H417" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I417" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="418" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="0" t="s">
+        <v>477</v>
+      </c>
       <c r="B418" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="H418" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I418" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="419" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B419" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="H419" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I419" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="420" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B420" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="H420" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I420" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="421" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B421" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="H421" s="0" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="I421" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="422" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B422" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="H422" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="I422" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="423" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B423" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="H423" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="I423" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="424" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B424" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="H424" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="I424" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B425" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="H425" s="0" t="s">
         <v>486</v>
       </c>
-      <c r="H425" s="0" t="s">
-        <v>473</v>
-      </c>
       <c r="I425" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6642,10 +6637,10 @@
         <v>487</v>
       </c>
       <c r="H426" s="0" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="I426" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6653,10 +6648,10 @@
         <v>488</v>
       </c>
       <c r="H427" s="0" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="I427" s="0" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6664,602 +6659,749 @@
         <v>489</v>
       </c>
       <c r="H428" s="0" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="I428" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B429" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="H429" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I429" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B430" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="H430" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I430" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B431" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="H431" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I431" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B432" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="H432" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I432" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B433" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="H433" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I433" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B434" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="H434" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I434" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B435" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="H435" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I435" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B436" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="H436" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I436" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B437" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="H437" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I437" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B438" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="H438" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I438" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B439" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="H439" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I439" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B440" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="H440" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I440" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B441" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="H441" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="I441" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B432" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="C432" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D432" s="0" t="s">
+      <c r="B445" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C445" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D445" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E432" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="F432" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="G432" s="0" t="n">
+      <c r="E445" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F445" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="G445" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H432" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I432" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J432" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="K432" s="0" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="0" t="s">
+      <c r="H445" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I445" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J445" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="K445" s="0" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A446" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B433" s="0" t="s">
-        <v>498</v>
-      </c>
-      <c r="C433" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D433" s="0" t="s">
+      <c r="B446" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="C446" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D446" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E433" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="F433" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="G433" s="0" t="n">
+      <c r="E446" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="F446" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="G446" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H433" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I433" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J433" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="K433" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="0" t="s">
+      <c r="H446" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I446" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J446" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="K446" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B434" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="C434" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D434" s="0" t="s">
+      <c r="B447" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C447" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D447" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E434" s="0" t="s">
+      <c r="E447" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="F447" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="G447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H447" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I447" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J447" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="K447" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B448" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="C448" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="F434" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="G434" s="0" t="n">
+      <c r="D448" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E448" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F448" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="G448" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H434" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I434" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J434" s="0" t="s">
-        <v>505</v>
-      </c>
-      <c r="K434" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B435" s="0" t="s">
-        <v>506</v>
-      </c>
-      <c r="C435" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D435" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E435" s="0" t="s">
+      <c r="H448" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="F435" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="G435" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H435" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I435" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J435" s="0" t="s">
+      <c r="I448" s="0" t="s">
         <v>508</v>
       </c>
-      <c r="K435" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B436" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="C436" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D436" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E436" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="F436" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="G436" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H436" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I436" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J436" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="K436" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B437" s="0" t="s">
-        <v>512</v>
-      </c>
-      <c r="C437" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D437" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E437" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="F437" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="G437" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H437" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I437" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J437" s="0" t="s">
-        <v>514</v>
-      </c>
-      <c r="K437" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B438" s="0" t="s">
+      <c r="J448" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="K448" s="0" t="s">
         <v>515</v>
-      </c>
-      <c r="C438" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D438" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E438" s="0" t="s">
-        <v>516</v>
-      </c>
-      <c r="F438" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="G438" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H438" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I438" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J438" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="K438" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B439" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="C439" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D439" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="E439" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="F439" s="0" t="s">
-        <v>520</v>
-      </c>
-      <c r="G439" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H439" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I439" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J439" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="K439" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B440" s="0" t="s">
-        <v>522</v>
-      </c>
-      <c r="C440" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D440" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="E440" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="F440" s="0" t="s">
-        <v>520</v>
-      </c>
-      <c r="G440" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H440" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I440" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J440" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="K440" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B441" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="C441" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D441" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="E441" s="0" t="s">
-        <v>527</v>
-      </c>
-      <c r="F441" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="G441" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H441" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I441" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J441" s="0" t="s">
-        <v>528</v>
-      </c>
-      <c r="K441" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B442" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="C442" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D442" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="E442" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="F442" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="G442" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H442" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I442" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J442" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="K442" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B443" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="C443" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="D443" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="E443" s="0" t="s">
-        <v>533</v>
-      </c>
-      <c r="F443" s="0" t="s">
-        <v>520</v>
-      </c>
-      <c r="G443" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H443" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="I443" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="J443" s="0" t="s">
-        <v>534</v>
-      </c>
-      <c r="K443" s="0" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="B449" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="C449" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D449" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E449" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="F449" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="G449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H449" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I449" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J449" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="K449" s="0" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A450" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="B450" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="C450" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D450" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E450" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="F450" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="G450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H450" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I450" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J450" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="K450" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="C451" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D451" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E451" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="F451" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="G451" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H451" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I451" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J451" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="K451" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B452" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="C452" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D452" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E452" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="F452" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="G452" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H452" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I452" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J452" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="K452" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B453" s="0" t="s">
         <v>535</v>
       </c>
-      <c r="H450" s="8" t="s">
+      <c r="C453" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D453" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E453" s="0" t="s">
         <v>536</v>
       </c>
-      <c r="I450" s="9" t="s">
+      <c r="F453" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="G453" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H453" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I453" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J453" s="0" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B451" s="0" t="s">
+      <c r="K453" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B454" s="0" t="s">
         <v>538</v>
       </c>
-      <c r="H451" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="I451" s="9" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B452" s="0" t="s">
+      <c r="C454" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D454" s="0" t="s">
         <v>539</v>
       </c>
-      <c r="H452" s="0" t="s">
+      <c r="E454" s="0" t="s">
         <v>540</v>
       </c>
-      <c r="I452" s="0" t="s">
-        <v>537</v>
+      <c r="F454" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="G454" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H454" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I454" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J454" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="K454" s="0" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="B455" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="H455" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="I455" s="9" t="s">
-        <v>60</v>
+      <c r="C455" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D455" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="E455" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="F455" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="G455" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H455" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I455" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J455" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="K455" s="0" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="B456" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H456" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I456" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B457" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="H457" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I457" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B458" s="0" t="s">
         <v>545</v>
       </c>
-      <c r="H458" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I458" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B459" s="0" t="s">
+      <c r="C456" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D456" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="E456" s="0" t="s">
         <v>546</v>
       </c>
-      <c r="H459" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I459" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B460" s="0" t="s">
+      <c r="F456" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="G456" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H456" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="I456" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="J456" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="H460" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I460" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B461" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="H461" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I461" s="9" t="s">
-        <v>60</v>
+      <c r="K456" s="0" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B462" s="0" t="s">
-        <v>549</v>
-      </c>
-      <c r="H462" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I462" s="9" t="s">
-        <v>60</v>
+      <c r="A462" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B463" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="H463" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="I463" s="8" t="s">
         <v>550</v>
-      </c>
-      <c r="H463" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I463" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B464" s="0" t="s">
         <v>551</v>
       </c>
-      <c r="H464" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I464" s="9" t="s">
-        <v>60</v>
+      <c r="H464" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="I464" s="8" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B465" s="0" t="s">
         <v>552</v>
       </c>
-      <c r="H465" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I465" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B466" s="0" t="s">
+      <c r="H465" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="H466" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="I466" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
+      <c r="I465" s="0" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B468" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="H468" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I468" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B469" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="H469" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I469" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B470" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="H470" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I470" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B471" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="H471" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I471" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B472" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="H472" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I472" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B473" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="H473" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I473" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B474" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="H474" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I474" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B475" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="H475" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I475" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B476" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="H476" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I476" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B477" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="H477" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I477" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B478" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="H478" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I478" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B479" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H479" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I479" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Remove mrfso from pre ignored list, #227.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="738">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1199,9 +1199,6 @@
   </si>
   <si>
     <t xml:space="preserve">zfullo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrfso</t>
   </si>
   <si>
     <t xml:space="preserve">burntFractionAll</t>
@@ -2470,8 +2467,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A399" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A404" activeCellId="0" sqref="A404"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B312" activeCellId="0" sqref="B312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6154,7 +6151,7 @@
         <v>393</v>
       </c>
       <c r="H312" s="0" t="s">
-        <v>269</v>
+        <v>394</v>
       </c>
       <c r="I312" s="0" t="s">
         <v>170</v>
@@ -6162,10 +6159,10 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H313" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I313" s="0" t="s">
         <v>170</v>
@@ -6173,10 +6170,10 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H314" s="0" t="s">
-        <v>397</v>
+        <v>306</v>
       </c>
       <c r="I314" s="0" t="s">
         <v>170</v>
@@ -6270,23 +6267,23 @@
         <v>170</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B323" s="0" t="s">
+    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B324" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="H324" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="H323" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="I323" s="0" t="s">
-        <v>170</v>
+      <c r="I324" s="0" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="H325" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I325" s="0" t="s">
         <v>350</v>
@@ -6294,10 +6291,10 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="0" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="H326" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I326" s="0" t="s">
         <v>350</v>
@@ -6305,10 +6302,10 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H327" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I327" s="0" t="s">
         <v>350</v>
@@ -6316,10 +6313,10 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H328" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I328" s="0" t="s">
         <v>350</v>
@@ -6327,10 +6324,10 @@
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H329" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I329" s="0" t="s">
         <v>350</v>
@@ -6338,10 +6335,10 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H330" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I330" s="0" t="s">
         <v>350</v>
@@ -6349,32 +6346,32 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H331" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I331" s="0" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B332" s="0" t="s">
-        <v>365</v>
-      </c>
-      <c r="H332" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="I332" s="0" t="s">
+    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B333" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="H333" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I333" s="0" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="0" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H334" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I334" s="0" t="s">
         <v>350</v>
@@ -6382,10 +6379,10 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H335" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I335" s="0" t="s">
         <v>350</v>
@@ -6393,35 +6390,35 @@
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H336" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I336" s="0" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B337" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="H337" s="2" t="s">
+    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B351" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="I337" s="0" t="s">
-        <v>350</v>
+      <c r="H351" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I351" s="6" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B352" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="H352" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="H352" s="5" t="s">
+      <c r="I352" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I352" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6429,10 +6426,10 @@
         <v>411</v>
       </c>
       <c r="H353" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I353" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I353" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6440,10 +6437,10 @@
         <v>412</v>
       </c>
       <c r="H354" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I354" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I354" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6451,10 +6448,10 @@
         <v>413</v>
       </c>
       <c r="H355" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I355" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I355" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6462,10 +6459,10 @@
         <v>414</v>
       </c>
       <c r="H356" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I356" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I356" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6473,10 +6470,10 @@
         <v>415</v>
       </c>
       <c r="H357" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I357" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I357" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6484,10 +6481,10 @@
         <v>416</v>
       </c>
       <c r="H358" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I358" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="I358" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6495,89 +6492,89 @@
         <v>417</v>
       </c>
       <c r="H359" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="I359" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="I359" s="6" t="s">
-        <v>410</v>
-      </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B360" s="0" t="s">
+      <c r="A360" s="0" t="s">
         <v>418</v>
-      </c>
-      <c r="H360" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="I360" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B361" s="2" t="s">
         <v>419</v>
+      </c>
+      <c r="C361" s="2"/>
+      <c r="D361" s="2"/>
+      <c r="H361" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="I361" s="0" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="B362" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="C362" s="2"/>
-      <c r="D362" s="2"/>
-      <c r="H362" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="I362" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="H363" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="I363" s="0" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B364" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="H364" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="I364" s="0" t="s">
         <v>424</v>
-      </c>
-      <c r="I364" s="0" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B365" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H365" s="0" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="I365" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="0" t="s">
-        <v>419</v>
-      </c>
       <c r="B366" s="0" t="s">
         <v>428</v>
       </c>
       <c r="H366" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="I366" s="0" t="s">
         <v>424</v>
-      </c>
-      <c r="I366" s="0" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6585,10 +6582,10 @@
         <v>429</v>
       </c>
       <c r="H367" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="I367" s="0" t="s">
         <v>424</v>
-      </c>
-      <c r="I367" s="0" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6596,76 +6593,76 @@
         <v>430</v>
       </c>
       <c r="H368" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="I368" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="I368" s="0" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B369" s="0" t="s">
+    </row>
+    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B374" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="H369" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="I369" s="0" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B375" s="0" t="s">
+      <c r="H374" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="H375" s="0" t="s">
+      <c r="I374" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B376" s="0" t="s">
         <v>433</v>
       </c>
-      <c r="I375" s="0" t="s">
-        <v>410</v>
+      <c r="H376" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="I376" s="0" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B377" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H377" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="I377" s="0" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B378" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H378" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I378" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B379" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H379" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I379" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="H380" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="H380" s="0" t="s">
-        <v>442</v>
-      </c>
       <c r="I380" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6673,10 +6670,10 @@
         <v>443</v>
       </c>
       <c r="H381" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I381" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6684,10 +6681,10 @@
         <v>444</v>
       </c>
       <c r="H382" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I382" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6695,43 +6692,43 @@
         <v>445</v>
       </c>
       <c r="H383" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="I383" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="H384" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I384" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B385" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="H385" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="I385" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B386" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H386" s="0" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="I386" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6739,313 +6736,313 @@
         <v>452</v>
       </c>
       <c r="H387" s="0" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="I387" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H388" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I388" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B389" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H389" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I389" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B390" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="H390" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="H390" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="I390" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>459</v>
+      </c>
       <c r="B391" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H391" s="0" t="s">
-        <v>458</v>
+        <v>432</v>
       </c>
       <c r="I391" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B392" s="0" t="s">
         <v>461</v>
       </c>
       <c r="H392" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I392" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="B393" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="H393" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="I393" s="0" t="s">
-        <v>410</v>
+        <v>459</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="B394" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="H394" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I394" s="0" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B395" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="H395" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="H395" s="0" t="s">
+      <c r="I395" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I395" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B396" s="0" t="s">
         <v>466</v>
       </c>
       <c r="H396" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I396" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I396" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B397" s="0" t="s">
         <v>467</v>
       </c>
       <c r="H397" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I397" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I397" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B398" s="0" t="s">
         <v>468</v>
       </c>
       <c r="H398" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I398" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I398" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B399" s="0" t="s">
         <v>469</v>
       </c>
       <c r="H399" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I399" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I399" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B400" s="0" t="s">
         <v>470</v>
       </c>
       <c r="H400" s="0" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="I400" s="0" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B401" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H401" s="0" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="I401" s="0" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B402" s="0" t="s">
         <v>474</v>
       </c>
       <c r="H402" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I402" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I402" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B403" s="0" t="s">
         <v>475</v>
       </c>
       <c r="H403" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I403" s="0" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B404" s="0" t="s">
         <v>476</v>
       </c>
       <c r="H404" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I404" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="0" t="s">
-        <v>460</v>
-      </c>
       <c r="B405" s="0" t="s">
         <v>477</v>
       </c>
       <c r="H405" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I405" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="0" t="s">
+        <v>478</v>
+      </c>
       <c r="B406" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H406" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I406" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B407" s="0" t="s">
         <v>480</v>
       </c>
       <c r="H407" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I407" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I407" s="0" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="B408" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="H408" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="I408" s="0" t="s">
-        <v>465</v>
+        <v>478</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
+      </c>
+      <c r="B409" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="H409" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I409" s="0" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B410" s="0" t="s">
         <v>482</v>
       </c>
       <c r="H410" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I410" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="I410" s="0" t="s">
-        <v>465</v>
-      </c>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="0" t="s">
-        <v>479</v>
-      </c>
       <c r="B411" s="0" t="s">
         <v>483</v>
       </c>
       <c r="H411" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I411" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I411" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7053,10 +7050,10 @@
         <v>484</v>
       </c>
       <c r="H412" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I412" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I412" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7064,32 +7061,32 @@
         <v>485</v>
       </c>
       <c r="H413" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="I413" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="I413" s="0" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B414" s="0" t="s">
+    </row>
+    <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B417" s="0" t="s">
         <v>486</v>
       </c>
-      <c r="H414" s="0" t="s">
+      <c r="H417" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="I417" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="I414" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B418" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="H418" s="0" t="s">
         <v>487</v>
       </c>
-      <c r="H418" s="0" t="s">
-        <v>488</v>
-      </c>
       <c r="I418" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7097,10 +7094,10 @@
         <v>489</v>
       </c>
       <c r="H419" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I419" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7108,10 +7105,10 @@
         <v>490</v>
       </c>
       <c r="H420" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I420" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7119,10 +7116,10 @@
         <v>491</v>
       </c>
       <c r="H421" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I421" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7130,10 +7127,10 @@
         <v>492</v>
       </c>
       <c r="H422" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I422" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7141,10 +7138,10 @@
         <v>493</v>
       </c>
       <c r="H423" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I423" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7152,21 +7149,21 @@
         <v>494</v>
       </c>
       <c r="H424" s="0" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="I424" s="0" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B425" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="H425" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="H425" s="0" t="s">
-        <v>496</v>
-      </c>
       <c r="I425" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7174,98 +7171,122 @@
         <v>497</v>
       </c>
       <c r="H426" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I426" s="0" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B427" s="0" t="s">
         <v>498</v>
       </c>
       <c r="H427" s="0" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="I427" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B428" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H428" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I428" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B429" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H429" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="I429" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B430" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H430" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="I430" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B431" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H431" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I431" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B432" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="H432" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="I432" s="0" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B433" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="H433" s="0" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="I433" s="0" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B434" s="0" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B437" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="H434" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="I434" s="0" t="s">
-        <v>473</v>
+      <c r="C437" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D437" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E437" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="F437" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="G437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H437" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I437" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="J437" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="K437" s="0" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7273,34 +7294,34 @@
         <v>46</v>
       </c>
       <c r="B438" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="C438" s="0" t="s">
         <v>512</v>
-      </c>
-      <c r="C438" s="0" t="s">
-        <v>513</v>
       </c>
       <c r="D438" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="G438" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H438" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I438" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I438" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J438" s="0" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="K438" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7308,34 +7329,34 @@
         <v>46</v>
       </c>
       <c r="B439" s="0" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="C439" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D439" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E439" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="F439" s="0" t="s">
         <v>521</v>
-      </c>
-      <c r="F439" s="0" t="s">
-        <v>522</v>
       </c>
       <c r="G439" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H439" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I439" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I439" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J439" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="K439" s="0" t="s">
         <v>523</v>
-      </c>
-      <c r="K439" s="0" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7343,34 +7364,34 @@
         <v>46</v>
       </c>
       <c r="B440" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C440" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D440" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E440" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F440" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G440" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H440" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I440" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I440" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J440" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="K440" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7378,34 +7399,34 @@
         <v>46</v>
       </c>
       <c r="B441" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C441" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D441" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G441" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H441" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I441" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I441" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J441" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="K441" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7413,34 +7434,34 @@
         <v>46</v>
       </c>
       <c r="B442" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C442" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D442" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G442" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H442" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I442" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I442" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J442" s="0" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="K442" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7448,34 +7469,34 @@
         <v>46</v>
       </c>
       <c r="B443" s="0" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C443" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D443" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G443" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H443" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I443" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I443" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J443" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="K443" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7483,34 +7504,34 @@
         <v>46</v>
       </c>
       <c r="B444" s="0" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="C444" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D444" s="0" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>522</v>
+        <v>541</v>
       </c>
       <c r="G444" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H444" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I444" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I444" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J444" s="0" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="K444" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7518,34 +7539,34 @@
         <v>46</v>
       </c>
       <c r="B445" s="0" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="C445" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D445" s="0" t="s">
         <v>209</v>
       </c>
       <c r="E445" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="F445" s="0" t="s">
         <v>541</v>
-      </c>
-      <c r="F445" s="0" t="s">
-        <v>542</v>
       </c>
       <c r="G445" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H445" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I445" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I445" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J445" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="K445" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7553,34 +7574,34 @@
         <v>46</v>
       </c>
       <c r="B446" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C446" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D446" s="0" t="s">
-        <v>209</v>
+        <v>547</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>542</v>
+        <v>512</v>
       </c>
       <c r="G446" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H446" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I446" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I446" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J446" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="K446" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7588,34 +7609,34 @@
         <v>46</v>
       </c>
       <c r="B447" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="C447" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D447" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="C447" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="D447" s="0" t="s">
-        <v>548</v>
-      </c>
       <c r="E447" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G447" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H447" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I447" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I447" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J447" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="K447" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7623,115 +7644,91 @@
         <v>46</v>
       </c>
       <c r="B448" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C448" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D448" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>513</v>
+        <v>541</v>
       </c>
       <c r="G448" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H448" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="I448" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="I448" s="0" t="s">
-        <v>517</v>
-      </c>
       <c r="J448" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="K448" s="0" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="0" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B449" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="C449" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="D449" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E449" s="0" t="s">
-        <v>555</v>
-      </c>
-      <c r="F449" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="G449" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H449" s="0" t="s">
-        <v>516</v>
-      </c>
-      <c r="I449" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="J449" s="0" t="s">
+    </row>
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B455" s="0" t="s">
         <v>556</v>
       </c>
-      <c r="K449" s="0" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="0" t="s">
-        <v>46</v>
+      <c r="H455" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="I455" s="8" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B456" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="H456" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="H456" s="7" t="s">
+      <c r="I456" s="8" t="s">
         <v>558</v>
-      </c>
-      <c r="I456" s="8" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B457" s="0" t="s">
         <v>560</v>
       </c>
-      <c r="H457" s="7" t="s">
+      <c r="H457" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="I457" s="0" t="s">
         <v>558</v>
       </c>
-      <c r="I457" s="8" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B458" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="H458" s="0" t="s">
+    </row>
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B460" s="0" t="s">
         <v>562</v>
       </c>
-      <c r="I458" s="0" t="s">
-        <v>559</v>
+      <c r="H460" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="I460" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B461" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="H461" s="9" t="s">
         <v>563</v>
-      </c>
-      <c r="H461" s="9" t="s">
-        <v>564</v>
       </c>
       <c r="I461" s="8" t="s">
         <v>60</v>
@@ -7742,7 +7739,7 @@
         <v>565</v>
       </c>
       <c r="H462" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I462" s="8" t="s">
         <v>60</v>
@@ -7753,7 +7750,7 @@
         <v>566</v>
       </c>
       <c r="H463" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I463" s="8" t="s">
         <v>60</v>
@@ -7764,7 +7761,7 @@
         <v>567</v>
       </c>
       <c r="H464" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I464" s="8" t="s">
         <v>60</v>
@@ -7775,7 +7772,7 @@
         <v>568</v>
       </c>
       <c r="H465" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I465" s="8" t="s">
         <v>60</v>
@@ -7786,7 +7783,7 @@
         <v>569</v>
       </c>
       <c r="H466" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I466" s="8" t="s">
         <v>60</v>
@@ -7797,7 +7794,7 @@
         <v>570</v>
       </c>
       <c r="H467" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I467" s="8" t="s">
         <v>60</v>
@@ -7808,7 +7805,7 @@
         <v>571</v>
       </c>
       <c r="H468" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I468" s="8" t="s">
         <v>60</v>
@@ -7819,7 +7816,7 @@
         <v>572</v>
       </c>
       <c r="H469" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I469" s="8" t="s">
         <v>60</v>
@@ -7830,7 +7827,7 @@
         <v>573</v>
       </c>
       <c r="H470" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I470" s="8" t="s">
         <v>60</v>
@@ -7841,21 +7838,45 @@
         <v>574</v>
       </c>
       <c r="H471" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I471" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B472" s="0" t="s">
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B474" s="0" t="s">
         <v>575</v>
       </c>
-      <c r="H472" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="I472" s="8" t="s">
-        <v>60</v>
+      <c r="C474" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E474" s="0" t="s">
+        <v>576</v>
+      </c>
+      <c r="F474" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="G474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H474" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="I474" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J474" s="0" t="s">
+        <v>578</v>
+      </c>
+      <c r="K474" s="0" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7863,7 +7884,7 @@
         <v>160</v>
       </c>
       <c r="B475" s="0" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="C475" s="0" t="n">
         <v>1</v>
@@ -7872,165 +7893,165 @@
         <v>41</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G475" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H475" s="0" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I475" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J475" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="K475" s="0" t="s">
         <v>579</v>
       </c>
-      <c r="K475" s="0" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B476" s="0" t="s">
-        <v>581</v>
-      </c>
-      <c r="C476" s="0" t="n">
+    </row>
+    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="C477" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D476" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E476" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="F476" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="G476" s="0" t="n">
+      <c r="D477" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="E477" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="F477" s="10" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="G477" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H476" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="I476" s="0" t="s">
+      <c r="H477" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="I477" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J476" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="K476" s="0" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B478" s="0" t="s">
-        <v>584</v>
-      </c>
-      <c r="C478" s="0" t="n">
+      <c r="J477" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="K477" s="0" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>589</v>
+      </c>
+      <c r="C479" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D478" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="E478" s="0" t="s">
-        <v>586</v>
-      </c>
-      <c r="F478" s="10" t="n">
-        <v>1E-009</v>
-      </c>
-      <c r="G478" s="0" t="n">
+      <c r="D479" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="E479" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="F479" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="G479" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H478" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="I478" s="0" t="s">
+      <c r="H479" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="I479" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J478" s="0" t="s">
-        <v>588</v>
-      </c>
-      <c r="K478" s="0" t="s">
-        <v>580</v>
+      <c r="J479" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="K479" s="0" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B480" s="0" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="C480" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D480" s="0" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E480" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="F480" s="0" t="s">
         <v>592</v>
-      </c>
-      <c r="F480" s="0" t="s">
-        <v>593</v>
       </c>
       <c r="G480" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H480" s="0" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I480" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J480" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="K480" s="0" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="0" t="s">
-        <v>589</v>
-      </c>
-      <c r="B481" s="0" t="s">
-        <v>595</v>
-      </c>
-      <c r="C481" s="0" t="n">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="C482" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D481" s="0" t="s">
-        <v>591</v>
-      </c>
-      <c r="E481" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="F481" s="0" t="s">
-        <v>593</v>
-      </c>
-      <c r="G481" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H481" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="I481" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J481" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="K481" s="0" t="s">
-        <v>580</v>
+      <c r="D482" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E482" s="0" t="s">
+        <v>598</v>
+      </c>
+      <c r="F482" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="G482" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H482" s="0" t="s">
+        <v>601</v>
+      </c>
+      <c r="I482" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="J482" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="K482" s="0" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8038,7 +8059,7 @@
         <v>44</v>
       </c>
       <c r="B483" s="0" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
       <c r="C483" s="0" t="n">
         <v>1</v>
@@ -8047,25 +8068,25 @@
         <v>13</v>
       </c>
       <c r="E483" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="F483" s="0" t="s">
         <v>599</v>
       </c>
-      <c r="F483" s="0" t="s">
+      <c r="G483" s="0" t="s">
         <v>600</v>
       </c>
-      <c r="G483" s="0" t="s">
-        <v>601</v>
-      </c>
       <c r="H483" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="I483" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I483" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J483" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="K483" s="0" t="s">
         <v>604</v>
-      </c>
-      <c r="K483" s="0" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8073,7 +8094,7 @@
         <v>44</v>
       </c>
       <c r="B484" s="0" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="C484" s="0" t="n">
         <v>1</v>
@@ -8082,25 +8103,25 @@
         <v>13</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="F484" s="0" t="s">
+        <v>611</v>
+      </c>
+      <c r="G484" s="0" t="s">
         <v>600</v>
       </c>
-      <c r="G484" s="0" t="s">
+      <c r="H484" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H484" s="0" t="s">
-        <v>608</v>
-      </c>
       <c r="I484" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J484" s="0" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="K484" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8108,7 +8129,7 @@
         <v>44</v>
       </c>
       <c r="B485" s="0" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="C485" s="0" t="n">
         <v>1</v>
@@ -8117,25 +8138,25 @@
         <v>13</v>
       </c>
       <c r="E485" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="F485" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="F485" s="0" t="s">
-        <v>612</v>
-      </c>
       <c r="G485" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H485" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="I485" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I485" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J485" s="0" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="K485" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8143,7 +8164,7 @@
         <v>44</v>
       </c>
       <c r="B486" s="0" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="C486" s="0" t="n">
         <v>1</v>
@@ -8152,25 +8173,25 @@
         <v>13</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>615</v>
-      </c>
-      <c r="F486" s="0" t="s">
-        <v>612</v>
+        <v>618</v>
+      </c>
+      <c r="F486" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G486" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H486" s="0" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="I486" s="0" t="s">
-        <v>603</v>
+        <v>620</v>
       </c>
       <c r="J486" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="K486" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8178,7 +8199,7 @@
         <v>44</v>
       </c>
       <c r="B487" s="0" t="s">
-        <v>618</v>
+        <v>168</v>
       </c>
       <c r="C487" s="0" t="n">
         <v>1</v>
@@ -8187,25 +8208,25 @@
         <v>13</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="F487" s="0" t="n">
-        <v>1</v>
+        <v>622</v>
+      </c>
+      <c r="F487" s="0" t="s">
+        <v>521</v>
       </c>
       <c r="G487" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H487" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H487" s="0" t="s">
-        <v>620</v>
-      </c>
       <c r="I487" s="0" t="s">
-        <v>621</v>
+        <v>602</v>
       </c>
       <c r="J487" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="K487" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8213,7 +8234,7 @@
         <v>44</v>
       </c>
       <c r="B488" s="0" t="s">
-        <v>168</v>
+        <v>624</v>
       </c>
       <c r="C488" s="0" t="n">
         <v>1</v>
@@ -8222,25 +8243,25 @@
         <v>13</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G488" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H488" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H488" s="0" t="s">
+      <c r="I488" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I488" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J488" s="0" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="K488" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8248,7 +8269,7 @@
         <v>44</v>
       </c>
       <c r="B489" s="0" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C489" s="0" t="n">
         <v>1</v>
@@ -8257,25 +8278,25 @@
         <v>13</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>522</v>
+        <v>541</v>
       </c>
       <c r="G489" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H489" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="I489" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I489" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J489" s="0" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="K489" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8283,7 +8304,7 @@
         <v>44</v>
       </c>
       <c r="B490" s="0" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C490" s="0" t="n">
         <v>1</v>
@@ -8292,25 +8313,25 @@
         <v>13</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G490" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H490" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H490" s="0" t="s">
-        <v>608</v>
-      </c>
       <c r="I490" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J490" s="0" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="K490" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8318,7 +8339,7 @@
         <v>44</v>
       </c>
       <c r="B491" s="0" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="C491" s="0" t="n">
         <v>1</v>
@@ -8327,25 +8348,25 @@
         <v>13</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G491" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H491" s="0" t="s">
+        <v>635</v>
+      </c>
+      <c r="I491" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I491" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J491" s="0" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="K491" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8353,7 +8374,7 @@
         <v>44</v>
       </c>
       <c r="B492" s="0" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="C492" s="0" t="n">
         <v>1</v>
@@ -8362,25 +8383,25 @@
         <v>13</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G492" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H492" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H492" s="0" t="s">
-        <v>636</v>
-      </c>
       <c r="I492" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J492" s="0" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="K492" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8388,7 +8409,7 @@
         <v>44</v>
       </c>
       <c r="B493" s="0" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="C493" s="0" t="n">
         <v>1</v>
@@ -8397,25 +8418,25 @@
         <v>13</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G493" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H493" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H493" s="0" t="s">
+      <c r="I493" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I493" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J493" s="0" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="K493" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8423,7 +8444,7 @@
         <v>44</v>
       </c>
       <c r="B494" s="0" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="C494" s="0" t="n">
         <v>1</v>
@@ -8432,25 +8453,25 @@
         <v>13</v>
       </c>
       <c r="E494" s="0" t="s">
-        <v>642</v>
-      </c>
-      <c r="F494" s="0" t="s">
-        <v>542</v>
+        <v>644</v>
+      </c>
+      <c r="F494" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G494" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H494" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H494" s="0" t="s">
+      <c r="I494" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I494" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J494" s="0" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="K494" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8458,7 +8479,7 @@
         <v>44</v>
       </c>
       <c r="B495" s="0" t="s">
-        <v>644</v>
+        <v>292</v>
       </c>
       <c r="C495" s="0" t="n">
         <v>1</v>
@@ -8467,25 +8488,25 @@
         <v>13</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>645</v>
-      </c>
-      <c r="F495" s="0" t="n">
-        <v>1</v>
+        <v>646</v>
+      </c>
+      <c r="F495" s="0" t="s">
+        <v>541</v>
       </c>
       <c r="G495" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H495" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="I495" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I495" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J495" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="K495" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8493,34 +8514,34 @@
         <v>44</v>
       </c>
       <c r="B496" s="0" t="s">
-        <v>292</v>
+        <v>648</v>
       </c>
       <c r="C496" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D496" s="0" t="s">
-        <v>13</v>
+        <v>649</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>647</v>
-      </c>
-      <c r="F496" s="0" t="s">
-        <v>542</v>
+        <v>650</v>
+      </c>
+      <c r="F496" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G496" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H496" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H496" s="0" t="s">
-        <v>608</v>
-      </c>
       <c r="I496" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J496" s="0" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="K496" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8528,34 +8549,34 @@
         <v>44</v>
       </c>
       <c r="B497" s="0" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="C497" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D497" s="0" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="F497" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G497" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H497" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H497" s="0" t="s">
+      <c r="I497" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I497" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J497" s="0" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="K497" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8563,34 +8584,34 @@
         <v>44</v>
       </c>
       <c r="B498" s="0" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="C498" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D498" s="0" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>654</v>
-      </c>
-      <c r="F498" s="0" t="n">
-        <v>1</v>
+        <v>657</v>
+      </c>
+      <c r="F498" s="0" t="s">
+        <v>658</v>
       </c>
       <c r="G498" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H498" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H498" s="0" t="s">
+      <c r="I498" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I498" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J498" s="0" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="K498" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8598,252 +8619,252 @@
         <v>44</v>
       </c>
       <c r="B499" s="0" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="C499" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D499" s="0" t="s">
-        <v>657</v>
+        <v>13</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="G499" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H499" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="H499" s="0" t="s">
+      <c r="I499" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="I499" s="0" t="s">
-        <v>603</v>
-      </c>
       <c r="J499" s="0" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="K499" s="0" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B500" s="0" t="s">
-        <v>661</v>
-      </c>
-      <c r="C500" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D500" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E500" s="0" t="s">
-        <v>662</v>
-      </c>
-      <c r="F500" s="0" t="s">
-        <v>663</v>
-      </c>
-      <c r="G500" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H500" s="0" t="s">
-        <v>602</v>
-      </c>
-      <c r="I500" s="0" t="s">
-        <v>603</v>
-      </c>
-      <c r="J500" s="0" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B502" s="0" t="s">
         <v>664</v>
       </c>
-      <c r="K500" s="0" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B503" s="0" t="s">
+      <c r="C502" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D502" s="0" t="s">
         <v>665</v>
       </c>
-      <c r="C503" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D503" s="0" t="s">
+      <c r="E502" s="0" t="s">
         <v>666</v>
       </c>
-      <c r="E503" s="0" t="s">
+      <c r="F502" s="0" t="s">
         <v>667</v>
       </c>
-      <c r="F503" s="0" t="s">
+      <c r="G502" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H502" s="0" t="s">
         <v>668</v>
       </c>
-      <c r="G503" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H503" s="0" t="s">
+      <c r="I502" s="0" t="s">
         <v>669</v>
       </c>
-      <c r="I503" s="0" t="s">
+      <c r="J502" s="0" t="s">
         <v>670</v>
       </c>
-      <c r="J503" s="0" t="s">
+      <c r="K502" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="K503" s="0" t="s">
+    </row>
+    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B504" s="0" t="s">
         <v>672</v>
+      </c>
+      <c r="C504" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D504" s="0" t="s">
+        <v>673</v>
+      </c>
+      <c r="E504" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="F504" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="G504" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H504" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="I504" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="J504" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="K504" s="0" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B505" s="0" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="C505" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D505" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>675</v>
-      </c>
-      <c r="F505" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="F505" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G505" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H505" s="0" t="s">
         <v>668</v>
       </c>
-      <c r="G505" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H505" s="0" t="s">
-        <v>676</v>
-      </c>
       <c r="I505" s="0" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J505" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="K505" s="0" t="s">
         <v>677</v>
-      </c>
-      <c r="K505" s="0" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B506" s="0" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="C506" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D506" s="0" t="s">
-        <v>680</v>
+        <v>13</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="F506" s="0" t="n">
-        <v>1</v>
+        <v>683</v>
+      </c>
+      <c r="F506" s="0" t="s">
+        <v>521</v>
       </c>
       <c r="G506" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H506" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="I506" s="0" t="s">
         <v>669</v>
       </c>
-      <c r="I506" s="0" t="s">
+      <c r="J506" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="K506" s="0" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B508" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="C508" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D508" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="E508" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="F508" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="G508" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H508" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="I508" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="J508" s="0" t="s">
         <v>670</v>
       </c>
-      <c r="J506" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="K506" s="0" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A507" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="B507" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="C507" s="0" t="n">
+      <c r="K508" s="0" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="B512" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="C512" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D507" s="0" t="s">
+      <c r="D512" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E507" s="0" t="s">
-        <v>684</v>
-      </c>
-      <c r="F507" s="0" t="s">
-        <v>522</v>
-      </c>
-      <c r="G507" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H507" s="0" t="s">
-        <v>669</v>
-      </c>
-      <c r="I507" s="0" t="s">
-        <v>670</v>
-      </c>
-      <c r="J507" s="0" t="s">
-        <v>685</v>
-      </c>
-      <c r="K507" s="0" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B509" s="0" t="s">
-        <v>665</v>
-      </c>
-      <c r="C509" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D509" s="0" t="s">
-        <v>687</v>
-      </c>
-      <c r="E509" s="0" t="s">
-        <v>667</v>
-      </c>
-      <c r="F509" s="0" t="s">
-        <v>668</v>
-      </c>
-      <c r="G509" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H509" s="0" t="s">
-        <v>669</v>
-      </c>
-      <c r="I509" s="0" t="s">
-        <v>670</v>
-      </c>
-      <c r="J509" s="0" t="s">
-        <v>671</v>
-      </c>
-      <c r="K509" s="0" t="s">
-        <v>672</v>
+      <c r="E512" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="F512" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="G512" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H512" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="I512" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="J512" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="K512" s="0" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B513" s="0" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="C513" s="0" t="n">
         <v>2</v>
@@ -8852,68 +8873,68 @@
         <v>13</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>690</v>
+        <v>521</v>
       </c>
       <c r="G513" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H513" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I513" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J513" s="0" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="K513" s="0" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B514" s="0" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="C514" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D514" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>522</v>
+        <v>698</v>
       </c>
       <c r="G514" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H514" s="0" t="s">
-        <v>179</v>
+        <v>699</v>
       </c>
       <c r="I514" s="0" t="s">
-        <v>410</v>
+        <v>700</v>
       </c>
       <c r="J514" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="K514" s="0" t="s">
         <v>695</v>
-      </c>
-      <c r="K514" s="0" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B515" s="0" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="C515" s="0" t="n">
         <v>3</v>
@@ -8922,339 +8943,305 @@
         <v>13</v>
       </c>
       <c r="E515" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="F515" s="0" t="s">
         <v>698</v>
       </c>
-      <c r="F515" s="0" t="s">
-        <v>699</v>
-      </c>
       <c r="G515" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H515" s="0" t="s">
-        <v>700</v>
+        <v>179</v>
       </c>
       <c r="I515" s="0" t="s">
-        <v>701</v>
+        <v>409</v>
       </c>
       <c r="J515" s="0" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="K515" s="0" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A516" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="B516" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="C516" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D516" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E516" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="F516" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="G516" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H516" s="0" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="B517" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="C517" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D517" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="E517" s="0" t="s">
+        <v>707</v>
+      </c>
+      <c r="F517" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="G517" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H517" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="I516" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="J516" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="K516" s="0" t="s">
-        <v>696</v>
+      <c r="I517" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="J517" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="K517" s="0" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="0" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B518" s="0" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C518" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D518" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E518" s="0" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="F518" s="0" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G518" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H518" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I518" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J518" s="0" t="s">
-        <v>691</v>
+        <v>711</v>
       </c>
       <c r="K518" s="0" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B519" s="0" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="C519" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D519" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G519" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H519" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I519" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J519" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="K519" s="0" t="s">
         <v>712</v>
-      </c>
-      <c r="K519" s="0" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B520" s="0" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C520" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D520" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G520" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H520" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I520" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J520" s="0" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="K520" s="0" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B521" s="0" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C521" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D521" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G521" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H521" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I521" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J521" s="0" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="K521" s="0" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B522" s="0" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C522" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D522" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G522" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H522" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I522" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J522" s="0" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="K522" s="0" t="s">
-        <v>713</v>
+        <v>725</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="0" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B523" s="0" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="C523" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D523" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G523" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H523" s="0" t="s">
         <v>179</v>
       </c>
       <c r="I523" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J523" s="0" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="K523" s="0" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A524" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="B524" s="0" t="s">
-        <v>727</v>
-      </c>
-      <c r="C524" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D524" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E524" s="0" t="s">
-        <v>728</v>
-      </c>
-      <c r="F524" s="0" t="s">
-        <v>690</v>
-      </c>
-      <c r="G524" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H524" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="I524" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="J524" s="0" t="s">
         <v>729</v>
       </c>
-      <c r="K524" s="0" t="s">
+    </row>
+    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="0" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="0" t="s">
+      <c r="B525" s="0" t="s">
         <v>731</v>
       </c>
-      <c r="B526" s="0" t="s">
+      <c r="C525" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D525" s="0" t="s">
         <v>732</v>
       </c>
-      <c r="C526" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D526" s="0" t="s">
+      <c r="E525" s="0" t="s">
         <v>733</v>
       </c>
-      <c r="E526" s="0" t="s">
+      <c r="G525" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H525" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="G526" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="H526" s="0" t="s">
+      <c r="I525" s="0" t="s">
         <v>735</v>
       </c>
-      <c r="I526" s="0" t="s">
+      <c r="J525" s="0" t="s">
         <v>736</v>
       </c>
-      <c r="J526" s="0" t="s">
+      <c r="K525" s="0" t="s">
         <v>737</v>
       </c>
-      <c r="K526" s="0" t="s">
-        <v>738</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add co2Clim & co2massClim to the ignored list including comment #320.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="793">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2401,6 +2401,42 @@
   </si>
   <si>
     <t xml:space="preserve">mass concentration of seasalt dry aerosol in air in model lowest layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude plev19 time2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mol mol-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in either IFS or TM5. With a lot of effort co2 output could be implemented in TM5, but on costs of performance. Moreover more issues remain in that case with this variable because it is in fact only requested in certain cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole fraction is used in the construction mole_fraction_of_X_in_Y, where X is a material constituent of Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CFMIP,CMIP,DAMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,PMIP,RFMIP,VolMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2massClim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Atmospheric Mass of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total atmospheric mass of Carbon Dioxide</t>
   </si>
 </sst>
 </file>
@@ -2596,8 +2632,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C512" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H541" activeCellId="0" sqref="H541:H542"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A533" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I546" activeCellId="0" sqref="I546:I547"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9699,6 +9735,78 @@
       </c>
       <c r="K542" s="0" t="s">
         <v>516</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A546" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B546" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C546" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D546" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="E546" s="0" t="s">
+        <v>783</v>
+      </c>
+      <c r="F546" s="0" t="s">
+        <v>784</v>
+      </c>
+      <c r="G546" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H546" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="I546" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J546" s="0" t="s">
+        <v>786</v>
+      </c>
+      <c r="K546" s="0" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A547" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B547" s="0" t="s">
+        <v>788</v>
+      </c>
+      <c r="C547" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D547" s="0" t="s">
+        <v>789</v>
+      </c>
+      <c r="E547" s="0" t="s">
+        <v>790</v>
+      </c>
+      <c r="F547" s="0" t="s">
+        <v>791</v>
+      </c>
+      <c r="G547" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ddf060894b16cf89e906ecfedbba4ffb.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H547" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="I547" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J547" s="0" t="s">
+        <v>792</v>
+      </c>
+      <c r="K547" s="0" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add hfibthermds to the pre ignored list #387.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="797">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1472,6 +1472,18 @@
   </si>
   <si>
     <t xml:space="preserve">difvmfdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfibthermds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA.  #387 and issue 595 at e-earth portal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.  The specification of a physical process by the phrase due_to_process means that the quantity named is a  single term in a sum of terms which together compose the general quantity  named by omitting the phrase.  ' Iceberg thermodynamics' refers to the addition or subtraction of mass due to surface and basal fluxes, i.e., due to melting, sublimation and fusion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,OMIP,VolMIP</t>
   </si>
   <si>
     <t xml:space="preserve">chldiaz</t>
@@ -2632,8 +2644,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A533" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I546" activeCellId="0" sqref="I546:I547"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A393" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H413" activeCellId="0" sqref="H413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7210,23 +7222,32 @@
         <v>462</v>
       </c>
     </row>
-    <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B415" s="0" t="s">
+    <row r="413" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B413" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="H415" s="0" t="s">
+      <c r="H413" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="I415" s="0" t="s">
-        <v>462</v>
+      <c r="I413" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J413" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="K413" s="3" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B416" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="H416" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I416" s="0" t="s">
         <v>462</v>
@@ -7234,10 +7255,10 @@
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B417" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="H417" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I417" s="0" t="s">
         <v>462</v>
@@ -7245,10 +7266,10 @@
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B418" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="H418" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I418" s="0" t="s">
         <v>462</v>
@@ -7256,10 +7277,10 @@
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B419" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="H419" s="0" t="s">
         <v>489</v>
-      </c>
-      <c r="H419" s="0" t="s">
-        <v>485</v>
       </c>
       <c r="I419" s="0" t="s">
         <v>462</v>
@@ -7267,10 +7288,10 @@
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B420" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="H420" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I420" s="0" t="s">
         <v>462</v>
@@ -7278,10 +7299,10 @@
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B421" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="H421" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I421" s="0" t="s">
         <v>462</v>
@@ -7289,21 +7310,21 @@
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B422" s="0" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="H422" s="0" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="I422" s="0" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B423" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="H423" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="I423" s="0" t="s">
         <v>470</v>
@@ -7311,18 +7332,18 @@
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B424" s="0" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="H424" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="I424" s="0" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B425" s="0" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="H425" s="0" t="s">
         <v>497</v>
@@ -7333,10 +7354,10 @@
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B426" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="H426" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="I426" s="0" t="s">
         <v>470</v>
@@ -7344,10 +7365,10 @@
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B427" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="H427" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="I427" s="0" t="s">
         <v>470</v>
@@ -7355,10 +7376,10 @@
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B428" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="H428" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="I428" s="0" t="s">
         <v>470</v>
@@ -7366,10 +7387,10 @@
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B429" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="H429" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="I429" s="0" t="s">
         <v>470</v>
@@ -7377,59 +7398,35 @@
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B430" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="H430" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="I430" s="0" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B431" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="H431" s="0" t="s">
-        <v>493</v>
+        <v>511</v>
       </c>
       <c r="I431" s="0" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B435" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="C435" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="D435" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E435" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="F435" s="0" t="s">
+    <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B432" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="G435" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H435" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="I435" s="0" t="s">
-        <v>514</v>
-      </c>
-      <c r="J435" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="K435" s="0" t="s">
-        <v>516</v>
+      <c r="H432" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="I432" s="0" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7437,34 +7434,34 @@
         <v>46</v>
       </c>
       <c r="B436" s="0" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C436" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D436" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E436" s="0" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F436" s="0" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="G436" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H436" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I436" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J436" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="K436" s="0" t="s">
         <v>520</v>
-      </c>
-      <c r="K436" s="0" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7472,34 +7469,34 @@
         <v>46</v>
       </c>
       <c r="B437" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C437" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D437" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E437" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="F437" s="0" t="s">
         <v>523</v>
-      </c>
-      <c r="F437" s="0" t="s">
-        <v>519</v>
       </c>
       <c r="G437" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H437" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I437" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J437" s="0" t="s">
         <v>524</v>
       </c>
       <c r="K437" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7507,34 +7504,34 @@
         <v>46</v>
       </c>
       <c r="B438" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C438" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D438" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="G438" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H438" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I438" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J438" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="K438" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7542,34 +7539,34 @@
         <v>46</v>
       </c>
       <c r="B439" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C439" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D439" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="G439" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H439" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I439" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J439" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="K439" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7577,34 +7574,34 @@
         <v>46</v>
       </c>
       <c r="B440" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C440" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D440" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E440" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F440" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="G440" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H440" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I440" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J440" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="K440" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7612,34 +7609,34 @@
         <v>46</v>
       </c>
       <c r="B441" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C441" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D441" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="G441" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H441" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I441" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J441" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="K441" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7647,34 +7644,34 @@
         <v>46</v>
       </c>
       <c r="B442" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C442" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D442" s="0" t="s">
-        <v>209</v>
+        <v>13</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="G442" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H442" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I442" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J442" s="0" t="s">
         <v>540</v>
       </c>
       <c r="K442" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7685,7 +7682,7 @@
         <v>541</v>
       </c>
       <c r="C443" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D443" s="0" t="s">
         <v>209</v>
@@ -7694,22 +7691,22 @@
         <v>542</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="G443" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H443" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I443" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J443" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="K443" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7717,34 +7714,34 @@
         <v>46</v>
       </c>
       <c r="B444" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C444" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D444" s="0" t="s">
-        <v>545</v>
+        <v>209</v>
       </c>
       <c r="E444" s="0" t="s">
         <v>546</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>510</v>
+        <v>543</v>
       </c>
       <c r="G444" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H444" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I444" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J444" s="0" t="s">
         <v>547</v>
       </c>
       <c r="K444" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7755,31 +7752,31 @@
         <v>548</v>
       </c>
       <c r="C445" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D445" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="G445" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H445" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I445" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="J445" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="K445" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7787,91 +7784,115 @@
         <v>46</v>
       </c>
       <c r="B446" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C446" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D446" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>539</v>
+        <v>514</v>
       </c>
       <c r="G446" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H446" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I446" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="J446" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="K446" s="0" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B447" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="C447" s="0" t="s">
         <v>514</v>
       </c>
-      <c r="J446" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="K446" s="0" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="0" t="s">
+      <c r="D447" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="E447" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="F447" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="G447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H447" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="I447" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="J447" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="K447" s="0" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="0" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B453" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="H453" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="I453" s="8" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B454" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="H454" s="7" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="I454" s="8" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B455" s="0" t="s">
-        <v>558</v>
-      </c>
-      <c r="H455" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="H455" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="I455" s="0" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B458" s="0" t="s">
+      <c r="I455" s="8" t="s">
         <v>560</v>
       </c>
-      <c r="H458" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="I458" s="8" t="s">
-        <v>60</v>
+    </row>
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B456" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="H456" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="I456" s="0" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B459" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="H459" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I459" s="8" t="s">
         <v>60</v>
@@ -7879,10 +7900,10 @@
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B460" s="0" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="H460" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I460" s="8" t="s">
         <v>60</v>
@@ -7890,10 +7911,10 @@
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B461" s="0" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="H461" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I461" s="8" t="s">
         <v>60</v>
@@ -7901,10 +7922,10 @@
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B462" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="H462" s="9" t="s">
         <v>565</v>
-      </c>
-      <c r="H462" s="9" t="s">
-        <v>561</v>
       </c>
       <c r="I462" s="8" t="s">
         <v>60</v>
@@ -7912,10 +7933,10 @@
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B463" s="0" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="H463" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I463" s="8" t="s">
         <v>60</v>
@@ -7923,10 +7944,10 @@
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B464" s="0" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="H464" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I464" s="8" t="s">
         <v>60</v>
@@ -7934,10 +7955,10 @@
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B465" s="0" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="H465" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I465" s="8" t="s">
         <v>60</v>
@@ -7945,10 +7966,10 @@
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B466" s="0" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="H466" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I466" s="8" t="s">
         <v>60</v>
@@ -7956,10 +7977,10 @@
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B467" s="0" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="H467" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I467" s="8" t="s">
         <v>60</v>
@@ -7967,10 +7988,10 @@
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B468" s="0" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="H468" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I468" s="8" t="s">
         <v>60</v>
@@ -7978,48 +7999,24 @@
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B469" s="0" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="H469" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I469" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B472" s="0" t="s">
-        <v>573</v>
-      </c>
-      <c r="C472" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D472" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E472" s="0" t="s">
-        <v>574</v>
-      </c>
-      <c r="F472" s="0" t="s">
-        <v>512</v>
-      </c>
-      <c r="G472" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H472" s="0" t="s">
-        <v>575</v>
-      </c>
-      <c r="I472" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J472" s="0" t="s">
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B470" s="0" t="s">
         <v>576</v>
       </c>
-      <c r="K472" s="0" t="s">
-        <v>577</v>
+      <c r="H470" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="I470" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8027,7 +8024,7 @@
         <v>160</v>
       </c>
       <c r="B473" s="0" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C473" s="0" t="n">
         <v>1</v>
@@ -8036,16 +8033,16 @@
         <v>41</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="G473" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H473" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="I473" s="0" t="s">
         <v>34</v>
@@ -8054,147 +8051,147 @@
         <v>580</v>
       </c>
       <c r="K473" s="0" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="0" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="C474" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E474" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="F474" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="G474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H474" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="I474" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J474" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="K474" s="0" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B475" s="0" t="s">
+      <c r="B476" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="C476" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D476" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="E476" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="F476" s="10" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="G476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H476" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="I476" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J476" s="0" t="s">
+        <v>589</v>
+      </c>
+      <c r="K476" s="0" t="s">
         <v>581</v>
-      </c>
-      <c r="C475" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D475" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="E475" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="F475" s="10" t="n">
-        <v>1E-009</v>
-      </c>
-      <c r="G475" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H475" s="0" t="s">
-        <v>584</v>
-      </c>
-      <c r="I475" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J475" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="K475" s="0" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="0" t="s">
-        <v>586</v>
-      </c>
-      <c r="B477" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="C477" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D477" s="0" t="s">
-        <v>588</v>
-      </c>
-      <c r="E477" s="0" t="s">
-        <v>589</v>
-      </c>
-      <c r="F477" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="G477" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H477" s="0" t="s">
-        <v>575</v>
-      </c>
-      <c r="I477" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J477" s="0" t="s">
-        <v>591</v>
-      </c>
-      <c r="K477" s="0" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="0" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="B478" s="0" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C478" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D478" s="0" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="E478" s="0" t="s">
         <v>593</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="G478" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H478" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="I478" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J478" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="K478" s="0" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="C479" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D479" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="E479" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="F479" s="0" t="s">
         <v>594</v>
       </c>
-      <c r="K478" s="0" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B480" s="0" t="s">
-        <v>595</v>
-      </c>
-      <c r="C480" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D480" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E480" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="F480" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="G480" s="0" t="s">
+      <c r="G479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H479" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="I479" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J479" s="0" t="s">
         <v>598</v>
       </c>
-      <c r="H480" s="0" t="s">
-        <v>599</v>
-      </c>
-      <c r="I480" s="0" t="s">
-        <v>600</v>
-      </c>
-      <c r="J480" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="K480" s="0" t="s">
-        <v>602</v>
+      <c r="K479" s="0" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8202,7 +8199,7 @@
         <v>44</v>
       </c>
       <c r="B481" s="0" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C481" s="0" t="n">
         <v>1</v>
@@ -8211,25 +8208,25 @@
         <v>13</v>
       </c>
       <c r="E481" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="F481" s="0" t="s">
+        <v>601</v>
+      </c>
+      <c r="G481" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H481" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="I481" s="0" t="s">
         <v>604</v>
       </c>
-      <c r="F481" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="G481" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H481" s="0" t="s">
+      <c r="J481" s="0" t="s">
         <v>605</v>
       </c>
-      <c r="I481" s="0" t="s">
-        <v>600</v>
-      </c>
-      <c r="J481" s="0" t="s">
+      <c r="K481" s="0" t="s">
         <v>606</v>
-      </c>
-      <c r="K481" s="0" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8249,22 +8246,22 @@
         <v>608</v>
       </c>
       <c r="F482" s="0" t="s">
+        <v>601</v>
+      </c>
+      <c r="G482" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H482" s="0" t="s">
         <v>609</v>
       </c>
-      <c r="G482" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H482" s="0" t="s">
-        <v>599</v>
-      </c>
       <c r="I482" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J482" s="0" t="s">
         <v>610</v>
       </c>
       <c r="K482" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8284,22 +8281,22 @@
         <v>612</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="G483" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H483" s="0" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="I483" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J483" s="0" t="s">
         <v>614</v>
       </c>
       <c r="K483" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8318,23 +8315,23 @@
       <c r="E484" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="F484" s="0" t="n">
-        <v>1</v>
+      <c r="F484" s="0" t="s">
+        <v>613</v>
       </c>
       <c r="G484" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H484" s="0" t="s">
         <v>617</v>
       </c>
       <c r="I484" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="J484" s="0" t="s">
         <v>618</v>
       </c>
-      <c r="J484" s="0" t="s">
-        <v>619</v>
-      </c>
       <c r="K484" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8342,7 +8339,7 @@
         <v>44</v>
       </c>
       <c r="B485" s="0" t="s">
-        <v>168</v>
+        <v>619</v>
       </c>
       <c r="C485" s="0" t="n">
         <v>1</v>
@@ -8353,23 +8350,23 @@
       <c r="E485" s="0" t="s">
         <v>620</v>
       </c>
-      <c r="F485" s="0" t="s">
-        <v>519</v>
+      <c r="F485" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G485" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H485" s="0" t="s">
-        <v>599</v>
+        <v>621</v>
       </c>
       <c r="I485" s="0" t="s">
-        <v>600</v>
+        <v>622</v>
       </c>
       <c r="J485" s="0" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="K485" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8377,7 +8374,7 @@
         <v>44</v>
       </c>
       <c r="B486" s="0" t="s">
-        <v>622</v>
+        <v>168</v>
       </c>
       <c r="C486" s="0" t="n">
         <v>1</v>
@@ -8386,25 +8383,25 @@
         <v>13</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="G486" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H486" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="I486" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J486" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="K486" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8412,7 +8409,7 @@
         <v>44</v>
       </c>
       <c r="B487" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C487" s="0" t="n">
         <v>1</v>
@@ -8421,25 +8418,25 @@
         <v>13</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="G487" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H487" s="0" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I487" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J487" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="K487" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8447,7 +8444,7 @@
         <v>44</v>
       </c>
       <c r="B488" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C488" s="0" t="n">
         <v>1</v>
@@ -8456,25 +8453,25 @@
         <v>13</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="G488" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H488" s="0" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="I488" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J488" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="K488" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8482,7 +8479,7 @@
         <v>44</v>
       </c>
       <c r="B489" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C489" s="0" t="n">
         <v>1</v>
@@ -8491,25 +8488,25 @@
         <v>13</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="G489" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H489" s="0" t="s">
-        <v>633</v>
+        <v>603</v>
       </c>
       <c r="I489" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J489" s="0" t="s">
         <v>634</v>
       </c>
       <c r="K489" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8529,22 +8526,22 @@
         <v>636</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="G490" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H490" s="0" t="s">
-        <v>599</v>
+        <v>637</v>
       </c>
       <c r="I490" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J490" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="K490" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8552,7 +8549,7 @@
         <v>44</v>
       </c>
       <c r="B491" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C491" s="0" t="n">
         <v>1</v>
@@ -8561,25 +8558,25 @@
         <v>13</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="G491" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H491" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="I491" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J491" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="K491" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8587,7 +8584,7 @@
         <v>44</v>
       </c>
       <c r="B492" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C492" s="0" t="n">
         <v>1</v>
@@ -8596,25 +8593,25 @@
         <v>13</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>642</v>
-      </c>
-      <c r="F492" s="0" t="n">
-        <v>1</v>
+        <v>643</v>
+      </c>
+      <c r="F492" s="0" t="s">
+        <v>543</v>
       </c>
       <c r="G492" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H492" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="I492" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J492" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K492" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8622,7 +8619,7 @@
         <v>44</v>
       </c>
       <c r="B493" s="0" t="s">
-        <v>290</v>
+        <v>645</v>
       </c>
       <c r="C493" s="0" t="n">
         <v>1</v>
@@ -8631,25 +8628,25 @@
         <v>13</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>644</v>
-      </c>
-      <c r="F493" s="0" t="s">
-        <v>539</v>
+        <v>646</v>
+      </c>
+      <c r="F493" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G493" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H493" s="0" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I493" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J493" s="0" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="K493" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8657,34 +8654,34 @@
         <v>44</v>
       </c>
       <c r="B494" s="0" t="s">
-        <v>646</v>
+        <v>290</v>
       </c>
       <c r="C494" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D494" s="0" t="s">
-        <v>647</v>
+        <v>13</v>
       </c>
       <c r="E494" s="0" t="s">
         <v>648</v>
       </c>
-      <c r="F494" s="0" t="n">
-        <v>1</v>
+      <c r="F494" s="0" t="s">
+        <v>543</v>
       </c>
       <c r="G494" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H494" s="0" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="I494" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J494" s="0" t="s">
         <v>649</v>
       </c>
       <c r="K494" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8698,28 +8695,28 @@
         <v>1</v>
       </c>
       <c r="D495" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="F495" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G495" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H495" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="I495" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J495" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="K495" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8727,34 +8724,34 @@
         <v>44</v>
       </c>
       <c r="B496" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C496" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D496" s="0" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="E496" s="0" t="s">
         <v>655</v>
       </c>
-      <c r="F496" s="0" t="s">
+      <c r="F496" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G496" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H496" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="I496" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="J496" s="0" t="s">
         <v>656</v>
       </c>
-      <c r="G496" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H496" s="0" t="s">
-        <v>599</v>
-      </c>
-      <c r="I496" s="0" t="s">
-        <v>600</v>
-      </c>
-      <c r="J496" s="0" t="s">
-        <v>657</v>
-      </c>
       <c r="K496" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8762,13 +8759,13 @@
         <v>44</v>
       </c>
       <c r="B497" s="0" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C497" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D497" s="0" t="s">
-        <v>13</v>
+        <v>658</v>
       </c>
       <c r="E497" s="0" t="s">
         <v>659</v>
@@ -8777,54 +8774,54 @@
         <v>660</v>
       </c>
       <c r="G497" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H497" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="I497" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="J497" s="0" t="s">
         <v>661</v>
       </c>
       <c r="K497" s="0" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B498" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="C498" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D498" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E498" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="F498" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="G498" s="0" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B499" s="0" t="s">
-        <v>662</v>
-      </c>
-      <c r="C499" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="D499" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E499" s="0" t="s">
-        <v>663</v>
-      </c>
-      <c r="F499" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="G499" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H499" s="0" t="s">
+      <c r="H498" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="I498" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="J498" s="0" t="s">
         <v>665</v>
       </c>
-      <c r="I499" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J499" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="K499" s="0" t="s">
-        <v>667</v>
+      <c r="K498" s="0" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8832,104 +8829,104 @@
         <v>44</v>
       </c>
       <c r="B500" s="0" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C500" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D500" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="G500" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H500" s="0" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I500" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J500" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="K500" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="K500" s="0" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="0" t="s">
+    </row>
+    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B501" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="C501" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D501" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E501" s="0" t="s">
+        <v>673</v>
+      </c>
+      <c r="F501" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="G501" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H501" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="I501" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J501" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="K501" s="0" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B503" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="C503" s="0" t="n">
+      <c r="B504" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="C504" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D503" s="0" t="s">
-        <v>673</v>
-      </c>
-      <c r="E503" s="0" t="s">
-        <v>674</v>
-      </c>
-      <c r="F503" s="0" t="s">
-        <v>675</v>
-      </c>
-      <c r="G503" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H503" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="I503" s="0" t="s">
+      <c r="D504" s="0" t="s">
         <v>677</v>
       </c>
-      <c r="J503" s="0" t="s">
+      <c r="E504" s="0" t="s">
         <v>678</v>
       </c>
-      <c r="K503" s="0" t="s">
+      <c r="F504" s="0" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="B505" s="0" t="s">
+      <c r="G504" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H504" s="0" t="s">
         <v>680</v>
       </c>
-      <c r="C505" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D505" s="0" t="s">
+      <c r="I504" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="E505" s="0" t="s">
+      <c r="J504" s="0" t="s">
         <v>682</v>
       </c>
-      <c r="F505" s="0" t="s">
-        <v>675</v>
-      </c>
-      <c r="G505" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H505" s="0" t="s">
+      <c r="K504" s="0" t="s">
         <v>683</v>
-      </c>
-      <c r="I505" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="J505" s="0" t="s">
-        <v>684</v>
-      </c>
-      <c r="K505" s="0" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8937,34 +8934,34 @@
         <v>416</v>
       </c>
       <c r="B506" s="0" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C506" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D506" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="E506" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="F506" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="G506" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H506" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="E506" s="0" t="s">
+      <c r="I506" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="J506" s="0" t="s">
         <v>688</v>
       </c>
-      <c r="F506" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G506" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H506" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="I506" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="J506" s="0" t="s">
+      <c r="K506" s="0" t="s">
         <v>689</v>
-      </c>
-      <c r="K506" s="0" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8975,101 +8972,101 @@
         <v>690</v>
       </c>
       <c r="C507" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D507" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E507" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="F507" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G507" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H507" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="I507" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="J507" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="K507" s="0" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B508" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="C508" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D507" s="0" t="s">
+      <c r="D508" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E507" s="0" t="s">
-        <v>691</v>
-      </c>
-      <c r="F507" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="G507" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H507" s="0" t="s">
+      <c r="E508" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="F508" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="G508" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H508" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="I508" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="J508" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="K508" s="0" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B510" s="0" t="s">
         <v>676</v>
       </c>
-      <c r="I507" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="J507" s="0" t="s">
-        <v>692</v>
-      </c>
-      <c r="K507" s="0" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B509" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="C509" s="0" t="n">
+      <c r="C510" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D509" s="0" t="s">
-        <v>694</v>
-      </c>
-      <c r="E509" s="0" t="s">
-        <v>674</v>
-      </c>
-      <c r="F509" s="0" t="s">
-        <v>675</v>
-      </c>
-      <c r="G509" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H509" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="I509" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="J509" s="0" t="s">
+      <c r="D510" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="E510" s="0" t="s">
         <v>678</v>
       </c>
-      <c r="K509" s="0" t="s">
+      <c r="F510" s="0" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A513" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="B513" s="0" t="s">
-        <v>695</v>
-      </c>
-      <c r="C513" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D513" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E513" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="F513" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="G513" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H513" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="I513" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="J513" s="0" t="s">
-        <v>698</v>
-      </c>
-      <c r="K513" s="0" t="s">
-        <v>699</v>
+      <c r="G510" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H510" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="I510" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="J510" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="K510" s="0" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9077,7 +9074,7 @@
         <v>457</v>
       </c>
       <c r="B514" s="0" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C514" s="0" t="n">
         <v>2</v>
@@ -9086,13 +9083,13 @@
         <v>13</v>
       </c>
       <c r="E514" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="F514" s="0" t="s">
         <v>701</v>
       </c>
-      <c r="F514" s="0" t="s">
-        <v>519</v>
-      </c>
       <c r="G514" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H514" s="0" t="s">
         <v>179</v>
@@ -9115,7 +9112,7 @@
         <v>704</v>
       </c>
       <c r="C515" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D515" s="0" t="s">
         <v>13</v>
@@ -9124,22 +9121,22 @@
         <v>705</v>
       </c>
       <c r="F515" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="G515" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H515" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="I515" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="J515" s="0" t="s">
         <v>706</v>
       </c>
-      <c r="G515" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H515" s="0" t="s">
+      <c r="K515" s="0" t="s">
         <v>707</v>
-      </c>
-      <c r="I515" s="0" t="s">
-        <v>708</v>
-      </c>
-      <c r="J515" s="0" t="s">
-        <v>709</v>
-      </c>
-      <c r="K515" s="0" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9147,7 +9144,7 @@
         <v>457</v>
       </c>
       <c r="B516" s="0" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C516" s="0" t="n">
         <v>3</v>
@@ -9156,83 +9153,83 @@
         <v>13</v>
       </c>
       <c r="E516" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="F516" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="G516" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H516" s="0" t="s">
         <v>711</v>
       </c>
-      <c r="F516" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="G516" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H516" s="0" t="s">
+      <c r="I516" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="J516" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="K516" s="0" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B517" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="C517" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D517" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E517" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="F517" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="G517" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H517" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="I516" s="0" t="s">
+      <c r="I517" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="J516" s="0" t="s">
-        <v>712</v>
-      </c>
-      <c r="K516" s="0" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A518" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="B518" s="0" t="s">
-        <v>714</v>
-      </c>
-      <c r="C518" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D518" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="E518" s="0" t="s">
-        <v>715</v>
-      </c>
-      <c r="F518" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="G518" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H518" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="I518" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="J518" s="0" t="s">
-        <v>698</v>
-      </c>
-      <c r="K518" s="0" t="s">
+      <c r="J517" s="0" t="s">
         <v>716</v>
+      </c>
+      <c r="K517" s="0" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B519" s="0" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C519" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D519" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G519" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H519" s="0" t="s">
         <v>179</v>
@@ -9241,7 +9238,7 @@
         <v>407</v>
       </c>
       <c r="J519" s="0" t="s">
-        <v>719</v>
+        <v>702</v>
       </c>
       <c r="K519" s="0" t="s">
         <v>720</v>
@@ -9249,25 +9246,25 @@
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B520" s="0" t="s">
         <v>721</v>
       </c>
       <c r="C520" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D520" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E520" s="0" t="s">
         <v>722</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G520" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H520" s="0" t="s">
         <v>179</v>
@@ -9279,30 +9276,30 @@
         <v>723</v>
       </c>
       <c r="K520" s="0" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B521" s="0" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C521" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D521" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G521" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H521" s="0" t="s">
         <v>179</v>
@@ -9311,33 +9308,33 @@
         <v>407</v>
       </c>
       <c r="J521" s="0" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="K521" s="0" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B522" s="0" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C522" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D522" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G522" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H522" s="0" t="s">
         <v>179</v>
@@ -9346,33 +9343,33 @@
         <v>407</v>
       </c>
       <c r="J522" s="0" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="K522" s="0" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B523" s="0" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C523" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D523" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G523" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H523" s="0" t="s">
         <v>179</v>
@@ -9381,33 +9378,33 @@
         <v>407</v>
       </c>
       <c r="J523" s="0" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="K523" s="0" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B524" s="0" t="s">
         <v>734</v>
       </c>
       <c r="C524" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D524" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E524" s="0" t="s">
         <v>735</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G524" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H524" s="0" t="s">
         <v>179</v>
@@ -9422,111 +9419,111 @@
         <v>737</v>
       </c>
     </row>
-    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="0" t="s">
+    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="B525" s="0" t="s">
         <v>738</v>
       </c>
-      <c r="B526" s="0" t="s">
+      <c r="C525" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D525" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="E525" s="0" t="s">
         <v>739</v>
       </c>
-      <c r="C526" s="0" t="n">
+      <c r="F525" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="G525" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H525" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="I525" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="J525" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="K525" s="0" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="B527" s="0" t="s">
+        <v>743</v>
+      </c>
+      <c r="C527" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D526" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="E526" s="0" t="s">
-        <v>741</v>
-      </c>
-      <c r="G526" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H526" s="0" t="s">
-        <v>742</v>
-      </c>
-      <c r="I526" s="0" t="s">
-        <v>743</v>
-      </c>
-      <c r="J526" s="0" t="s">
+      <c r="D527" s="0" t="s">
         <v>744</v>
       </c>
-      <c r="K526" s="0" t="s">
+      <c r="E527" s="0" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="0" t="s">
+      <c r="G527" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H527" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="I527" s="0" t="s">
+        <v>747</v>
+      </c>
+      <c r="J527" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="K527" s="0" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="B530" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="C530" s="0" t="n">
+      <c r="B531" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="C531" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D530" s="0" t="s">
-        <v>747</v>
-      </c>
-      <c r="E530" s="0" t="s">
-        <v>748</v>
-      </c>
-      <c r="F530" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="G530" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H530" s="0" t="s">
-        <v>749</v>
-      </c>
-      <c r="I530" s="0" t="s">
+      <c r="D531" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="E531" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="F531" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="G531" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H531" s="0" t="s">
+        <v>753</v>
+      </c>
+      <c r="I531" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="J530" s="0" t="s">
-        <v>750</v>
-      </c>
-      <c r="K530" s="0" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="B532" s="0" t="s">
-        <v>751</v>
-      </c>
-      <c r="C532" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D532" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="E532" s="0" t="s">
-        <v>752</v>
-      </c>
-      <c r="F532" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="G532" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H532" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="I532" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="J532" s="0" t="s">
+      <c r="J531" s="0" t="s">
         <v>754</v>
       </c>
-      <c r="K532" s="0" t="s">
-        <v>716</v>
+      <c r="K531" s="0" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B533" s="0" t="s">
         <v>755</v>
@@ -9535,16 +9532,16 @@
         <v>1</v>
       </c>
       <c r="D533" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E533" s="0" t="s">
         <v>756</v>
       </c>
-      <c r="F533" s="0" t="n">
-        <v>1</v>
+      <c r="F533" s="0" t="s">
+        <v>701</v>
       </c>
       <c r="G533" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="H533" s="0" t="s">
         <v>757</v>
@@ -9556,79 +9553,78 @@
         <v>758</v>
       </c>
       <c r="K533" s="0" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A536" s="0" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="B534" s="0" t="s">
         <v>759</v>
       </c>
-      <c r="B536" s="0" t="s">
+      <c r="C534" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D534" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="E534" s="0" t="s">
         <v>760</v>
       </c>
-      <c r="C536" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="D536" s="0" t="s">
+      <c r="F534" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G534" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H534" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="I534" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="J534" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="K534" s="0" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A537" s="0" t="s">
+        <v>763</v>
+      </c>
+      <c r="B537" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="C537" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D537" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E536" s="0" t="s">
-        <v>761</v>
-      </c>
-      <c r="F536" s="0" t="s">
-        <v>512</v>
-      </c>
-      <c r="G536" s="0" t="str">
+      <c r="E537" s="0" t="s">
+        <v>765</v>
+      </c>
+      <c r="F537" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="G537" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H536" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="I536" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="J536" s="0" t="s">
-        <v>763</v>
-      </c>
-      <c r="K536" s="0" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B537" s="0" t="s">
-        <v>765</v>
-      </c>
-      <c r="C537" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="D537" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E537" s="0" t="s">
+      <c r="H537" s="3" t="s">
         <v>766</v>
-      </c>
-      <c r="F537" s="0" t="s">
-        <v>512</v>
-      </c>
-      <c r="G537" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590daf66-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H537" s="3" t="s">
-        <v>767</v>
       </c>
       <c r="I537" s="0" t="s">
         <v>60</v>
       </c>
       <c r="J537" s="0" t="s">
+        <v>767</v>
+      </c>
+      <c r="K537" s="0" t="s">
         <v>768</v>
-      </c>
-      <c r="K537" s="0" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9639,7 +9635,7 @@
         <v>769</v>
       </c>
       <c r="C538" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D538" s="0" t="s">
         <v>41</v>
@@ -9648,58 +9644,59 @@
         <v>770</v>
       </c>
       <c r="F538" s="0" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="G538" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590daf66-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H538" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="I538" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J538" s="0" t="s">
+        <v>772</v>
+      </c>
+      <c r="K538" s="0" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A539" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B539" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C539" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D539" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E539" s="0" t="s">
+        <v>774</v>
+      </c>
+      <c r="F539" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="G539" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H538" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="I538" s="0" t="s">
+      <c r="H539" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="I539" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="J538" s="0" t="s">
-        <v>771</v>
-      </c>
-      <c r="K538" s="0" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A541" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B541" s="0" t="s">
-        <v>772</v>
-      </c>
-      <c r="C541" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D541" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="E541" s="0" t="s">
-        <v>773</v>
-      </c>
-      <c r="F541" s="0" t="s">
-        <v>774</v>
-      </c>
-      <c r="G541" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H541" s="0" t="s">
+      <c r="J539" s="0" t="s">
         <v>775</v>
       </c>
-      <c r="I541" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="J541" s="0" t="s">
-        <v>776</v>
-      </c>
-      <c r="K541" s="0" t="s">
-        <v>516</v>
+      <c r="K539" s="0" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9707,25 +9704,25 @@
         <v>46</v>
       </c>
       <c r="B542" s="0" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C542" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D542" s="0" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
       <c r="E542" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="F542" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="F542" s="0" t="s">
+      <c r="G542" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H542" s="0" t="s">
         <v>779</v>
-      </c>
-      <c r="G542" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="H542" s="0" t="s">
-        <v>775</v>
       </c>
       <c r="I542" s="0" t="s">
         <v>246</v>
@@ -9734,43 +9731,42 @@
         <v>780</v>
       </c>
       <c r="K542" s="0" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A546" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B546" s="0" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B543" s="0" t="s">
         <v>781</v>
       </c>
-      <c r="C546" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="D546" s="0" t="s">
+      <c r="C543" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D543" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E543" s="0" t="s">
         <v>782</v>
       </c>
-      <c r="E546" s="0" t="s">
+      <c r="F543" s="0" t="s">
         <v>783</v>
       </c>
-      <c r="F546" s="0" t="s">
+      <c r="G543" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="H543" s="0" t="s">
+        <v>779</v>
+      </c>
+      <c r="I543" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="J543" s="0" t="s">
         <v>784</v>
       </c>
-      <c r="G546" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H546" s="0" t="s">
-        <v>785</v>
-      </c>
-      <c r="I546" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J546" s="0" t="s">
-        <v>786</v>
-      </c>
-      <c r="K546" s="0" t="s">
-        <v>787</v>
+      <c r="K543" s="0" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9778,38 +9774,73 @@
         <v>11</v>
       </c>
       <c r="B547" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="C547" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D547" s="0" t="s">
+        <v>786</v>
+      </c>
+      <c r="E547" s="0" t="s">
+        <v>787</v>
+      </c>
+      <c r="F547" s="0" t="s">
         <v>788</v>
       </c>
-      <c r="C547" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="D547" s="0" t="s">
+      <c r="G547" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H547" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="E547" s="0" t="s">
+      <c r="I547" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J547" s="0" t="s">
         <v>790</v>
       </c>
-      <c r="F547" s="0" t="s">
+      <c r="K547" s="0" t="s">
         <v>791</v>
       </c>
-      <c r="G547" s="0" t="str">
+    </row>
+    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A548" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B548" s="0" t="s">
+        <v>792</v>
+      </c>
+      <c r="C548" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D548" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="E548" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="F548" s="0" t="s">
+        <v>795</v>
+      </c>
+      <c r="G548" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ddf060894b16cf89e906ecfedbba4ffb.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H547" s="0" t="s">
-        <v>785</v>
-      </c>
-      <c r="I547" s="0" t="s">
+      <c r="H548" s="0" t="s">
+        <v>789</v>
+      </c>
+      <c r="I548" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="J547" s="0" t="s">
-        <v>792</v>
-      </c>
-      <c r="K547" s="0" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J548" s="0" t="s">
+        <v>796</v>
+      </c>
+      <c r="K548" s="0" t="s">
+        <v>791</v>
+      </c>
+    </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Identification of Ofx ugrido: to the pre-ignored list #554.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="772">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2362,6 +2362,18 @@
   </si>
   <si>
     <t xml:space="preserve">Percentage water content of soil by volume at the wilting point. The wilting point of soil is the water content below which plants cannot extract sufficient water to balance their loss through transpiration. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ofx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ugrido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UGRID Grid Specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEMO has a structured grid, so we do not need to provide this</t>
   </si>
 </sst>
 </file>
@@ -2617,8 +2629,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A285" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A305" activeCellId="0" sqref="A305"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A529" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H549" activeCellId="0" sqref="H549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9030,6 +9042,39 @@
       </c>
       <c r="K546" s="0" t="s">
         <v>547</v>
+      </c>
+    </row>
+    <row r="549" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A549" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="B549" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="C549" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D549" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="E549" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="G549" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/962e51dc-267b-11e7-96a5-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H549" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="I549" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J549" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="K549" s="3" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Identification of a few last missing variables: all added to the ignored list including comment #554.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="807">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2364,6 +2364,111 @@
     <t xml:space="preserve">Percentage water content of soil by volume at the wilting point. The wilting point of soil is the water content below which plants cannot extract sufficient water to balance their loss through transpiration. </t>
   </si>
   <si>
+    <t xml:space="preserve">LImon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pflw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liquid Water Content of Permafrost Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available from IFS-HTESSEL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco,Twan,Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*where land over land*, i.e., this is the total mass of liquid water contained within the permafrost layer within the land portion of a grid cell divided by the area of the land portion of the cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4MIP,CMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,VIACSAB,VolMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sootsn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snow Soot Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the entire land portion of the grid cell is considered, with snow soot content set to 0.0 in regions free of snow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cldncl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Droplet Number Concentration of Cloud Tops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This variable entered in a very late stage, and is only asked by VIACSAB. Therefore it is ignored. It potentially could be produced by a processing of some already implemented IFS - PEXTRA variables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Droplets are liquid only.  Report concentration 'as seen from space' over liquid cloudy portion of grid cell.  This is the value from uppermost model layer with liquid cloud or, if available, it is better to sum over all liquid cloud tops, no matter where they occur, as long as they are seen from the top of the atmosphere. Weight by total liquid cloud top fraction of  (as seen from TOA) each time sample when computing monthly mean.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cldnvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column Integrated Cloud Droplet Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This variable entered in a very late stage, and is only asked by VIACSAB. Therefore it is ignored. cdnc is available as monthly 3-D field from IFS PEXTRA (at least for AerChemMIP) from which the column integrated variable can be derived.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Droplets are liquid only.  Values are weighted by liquid cloud fraction in each layer when vertically integrating, and for monthly means the samples are weighted by total liquid cloud fraction (as seen from TOA).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loadso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load of SO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With additional coding in TM5 this variable could be produced by TM5, but because VIACSAB is only part of the joined EC-Earth3-AOGCM request and this configuration does not include TM5, this variable can be ignored. Moreover, mmrso4 is available for AerChemMIP from which loadso4 can be derived by users themselves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommi, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total dry mass of sulfate aerosol particles per unit area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loadss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load of Sea-Salt Aerosol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With additional coding in TM5 this variable could be produced by TM5, but because VIACSAB is only part of the joined EC-Earth3-AOGCM request and this configuration does not include TM5, this variable can be ignored. Moreover, mmrss is available for AerChemMIP from which loadss can be derived by users themselves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total dry mass of sea salt aerosol particles per unit area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw17O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO. According to the ping_ocean_DR1.00.27.xml file sw18O has a dummy status; confusingly the description of sw18O refers to 17O isotopes. But neither is available according to a search in the ping files.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio of abundance of oxygen-17 (17O) atoms to oxygen-16 (16O) atoms in sea water</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ofx</t>
   </si>
   <si>
@@ -2384,7 +2489,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2450,6 +2555,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2505,7 +2616,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2547,6 +2658,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2630,7 +2745,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A529" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H549" activeCellId="0" sqref="H549"/>
+      <selection pane="topLeft" activeCell="A548" activeCellId="0" sqref="548:548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9044,39 +9159,292 @@
         <v>547</v>
       </c>
     </row>
-    <row r="549" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A549" s="3" t="s">
+    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A550" s="0" t="s">
         <v>768</v>
       </c>
-      <c r="B549" s="3" t="s">
+      <c r="B550" s="0" t="s">
         <v>769</v>
       </c>
-      <c r="C549" s="3" t="s">
+      <c r="C550" s="0" t="s">
+        <v>770</v>
+      </c>
+      <c r="D550" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E550" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="F550" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="G550" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/67adc30ae1278d2ef6d696ba0e2c92e8.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H550" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="I550" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="J550" s="0" t="s">
+        <v>774</v>
+      </c>
+      <c r="K550" s="0" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A551" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="B551" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="C551" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="D551" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E551" s="0" t="s">
+        <v>778</v>
+      </c>
+      <c r="F551" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="G551" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d421b6923b396998106a8c1c66ea07f1.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H551" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="I551" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="J551" s="0" t="s">
+        <v>779</v>
+      </c>
+      <c r="K551" s="0" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A553" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B553" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C553" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D549" s="3" t="s">
+      <c r="D553" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E553" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="F553" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="G553" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/069ed8a3f93e92dab9e61f59b4d5338e.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H553" s="11" t="s">
+        <v>783</v>
+      </c>
+      <c r="I553" s="0" t="s">
+        <v>784</v>
+      </c>
+      <c r="J553" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="K553" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A554" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B554" s="0" t="s">
+        <v>786</v>
+      </c>
+      <c r="C554" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D554" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E554" s="0" t="s">
+        <v>787</v>
+      </c>
+      <c r="F554" s="0" t="s">
+        <v>788</v>
+      </c>
+      <c r="G554" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f946653cd518e221676f263a895c7852.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H554" s="11" t="s">
+        <v>789</v>
+      </c>
+      <c r="I554" s="0" t="s">
+        <v>784</v>
+      </c>
+      <c r="J554" s="0" t="s">
+        <v>790</v>
+      </c>
+      <c r="K554" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A555" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B555" s="0" t="s">
+        <v>791</v>
+      </c>
+      <c r="C555" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D555" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E555" s="0" t="s">
+        <v>792</v>
+      </c>
+      <c r="F555" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="G555" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H555" s="11" t="s">
+        <v>793</v>
+      </c>
+      <c r="I555" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="J555" s="0" t="s">
+        <v>795</v>
+      </c>
+      <c r="K555" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B556" s="0" t="s">
+        <v>796</v>
+      </c>
+      <c r="C556" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D556" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E556" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="F556" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="G556" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H556" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="I556" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="J556" s="0" t="s">
+        <v>799</v>
+      </c>
+      <c r="K556" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A557" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B557" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="C557" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D557" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="E557" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="F557" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="G557" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cbf-4d35-11e8-be0a-1c4d70487308.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H557" s="11" t="s">
+        <v>801</v>
+      </c>
+      <c r="I557" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J557" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="K557" s="0" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A559" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="B559" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="C559" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D559" s="0" t="s">
         <v>683</v>
       </c>
-      <c r="E549" s="3" t="s">
-        <v>770</v>
-      </c>
-      <c r="G549" s="3" t="str">
+      <c r="E559" s="0" t="s">
+        <v>805</v>
+      </c>
+      <c r="G559" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/962e51dc-267b-11e7-96a5-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H549" s="3" t="s">
-        <v>771</v>
-      </c>
-      <c r="I549" s="3" t="s">
+      <c r="H559" s="11" t="s">
+        <v>806</v>
+      </c>
+      <c r="I559" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J549" s="3" t="s">
+      <c r="J559" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="K549" s="3" t="s">
+      <c r="K559" s="0" t="s">
         <v>688</v>
       </c>
     </row>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Remove dissicnat & talknat from the pre ignored and ignored lists, they are now available #521.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="802">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1271,9 +1271,6 @@
   </si>
   <si>
     <t xml:space="preserve">phypico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">talknat</t>
   </si>
   <si>
     <t xml:space="preserve">difvtrbo</t>
@@ -2142,18 +2139,6 @@
     <t xml:space="preserve">The surface called 'surface' means the lower boundary of the atmosphere. The chemical formula for carbon dioxide is CO2. In ocean biogeochemistry models, a 'natural analogue' is used to simulate the effect on a modelled variable of imposing preindustrial atmospheric carbon dioxide concentrations, even when the model as a whole may be subjected to varying forcings. The partial pressure of a gaseous constituent of air is the pressure which it alone would exert with unchanged temperature and number of moles per unit volume. The partial pressure of a dissolved gas in sea water is the partial pressure in air with which it would be in equilibrium. The partial pressure difference between sea water and air is positive when the partial pressure of the dissolved gas in sea water is greater than the partial pressure in air.</t>
   </si>
   <si>
-    <t xml:space="preserve">dissicnat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural Dissolved Inorganic Carbon Concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Will be only for OMIP manually added: DIC_E3T/e3t in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved inorganic carbon (CO3+HCO3+H2CO3) concentration at preindustrial atmospheric xCO2</t>
-  </si>
-  <si>
     <t xml:space="preserve">phnat</t>
   </si>
   <si>
@@ -2489,7 +2474,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2555,12 +2540,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2616,7 +2595,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2658,10 +2637,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2744,8 +2719,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A529" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A548" activeCellId="0" sqref="548:548"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C369" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A389" activeCellId="0" sqref="A389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6431,14 +6406,14 @@
         <v>410</v>
       </c>
     </row>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B389" s="0" t="s">
+    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B390" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="H389" s="0" t="s">
+      <c r="H390" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="I389" s="0" t="s">
+      <c r="I390" s="0" t="s">
         <v>402</v>
       </c>
     </row>
@@ -6486,40 +6461,40 @@
         <v>402</v>
       </c>
     </row>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B395" s="0" t="s">
+    <row r="396" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B396" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="H395" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="I395" s="0" t="s">
+      <c r="H396" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="I396" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J396" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="K396" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B399" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="H399" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="I399" s="0" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="397" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B397" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="H397" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="I397" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J397" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="K397" s="3" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B400" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="H400" s="0" t="s">
         <v>427</v>
-      </c>
-      <c r="H400" s="0" t="s">
-        <v>428</v>
       </c>
       <c r="I400" s="0" t="s">
         <v>402</v>
@@ -6530,7 +6505,7 @@
         <v>429</v>
       </c>
       <c r="H401" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I401" s="0" t="s">
         <v>402</v>
@@ -6541,7 +6516,7 @@
         <v>430</v>
       </c>
       <c r="H402" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I402" s="0" t="s">
         <v>402</v>
@@ -6552,7 +6527,7 @@
         <v>431</v>
       </c>
       <c r="H403" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I403" s="0" t="s">
         <v>402</v>
@@ -6563,7 +6538,7 @@
         <v>432</v>
       </c>
       <c r="H404" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I404" s="0" t="s">
         <v>402</v>
@@ -6574,7 +6549,7 @@
         <v>433</v>
       </c>
       <c r="H405" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I405" s="0" t="s">
         <v>402</v>
@@ -6585,18 +6560,18 @@
         <v>434</v>
       </c>
       <c r="H406" s="0" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="I406" s="0" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B407" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="H407" s="0" t="s">
         <v>435</v>
-      </c>
-      <c r="H407" s="0" t="s">
-        <v>436</v>
       </c>
       <c r="I407" s="0" t="s">
         <v>410</v>
@@ -6607,18 +6582,18 @@
         <v>437</v>
       </c>
       <c r="H408" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I408" s="0" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="409" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B409" s="0" t="s">
         <v>438</v>
       </c>
       <c r="H409" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="I409" s="0" t="s">
         <v>410</v>
@@ -6626,10 +6601,10 @@
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B410" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H410" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I410" s="0" t="s">
         <v>410</v>
@@ -6637,10 +6612,10 @@
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B411" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H411" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I411" s="0" t="s">
         <v>410</v>
@@ -6648,10 +6623,10 @@
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B412" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H412" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I412" s="0" t="s">
         <v>410</v>
@@ -6659,10 +6634,10 @@
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B413" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H413" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I413" s="0" t="s">
         <v>410</v>
@@ -6670,460 +6645,460 @@
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B414" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H414" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I414" s="0" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B415" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="H415" s="0" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="I415" s="0" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="416" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B416" s="0" t="s">
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B419" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="H416" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="I416" s="0" t="s">
-        <v>410</v>
+      <c r="C419" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D419" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E419" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="F419" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="G419" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H419" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I419" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="J419" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="K419" s="0" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B420" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C420" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="C420" s="0" t="s">
+      <c r="D420" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D420" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E420" s="0" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="F420" s="0" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="G420" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H420" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I420" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I420" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J420" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="K420" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B421" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C421" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D421" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D421" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E421" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="F421" s="0" t="s">
         <v>462</v>
-      </c>
-      <c r="F421" s="0" t="s">
-        <v>463</v>
       </c>
       <c r="G421" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H421" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I421" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I421" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J421" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="K421" s="0" t="s">
         <v>464</v>
-      </c>
-      <c r="K421" s="0" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B422" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C422" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D422" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D422" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E422" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="F422" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G422" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H422" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I422" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I422" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J422" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="K422" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B423" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C423" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D423" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D423" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E423" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F423" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G423" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H423" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I423" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I423" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J423" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="K423" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B424" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C424" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D424" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D424" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E424" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F424" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G424" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H424" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I424" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I424" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J424" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="K424" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B425" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C425" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D425" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D425" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E425" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="F425" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G425" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H425" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I425" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I425" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J425" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="K425" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B426" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C426" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D426" s="0" t="s">
-        <v>454</v>
+        <v>481</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="F426" s="0" t="s">
-        <v>463</v>
+        <v>483</v>
       </c>
       <c r="G426" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H426" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I426" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I426" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J426" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="K426" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B427" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C427" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D427" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="C427" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D427" s="0" t="s">
-        <v>482</v>
-      </c>
       <c r="E427" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="F427" s="0" t="s">
         <v>483</v>
-      </c>
-      <c r="F427" s="0" t="s">
-        <v>484</v>
       </c>
       <c r="G427" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H427" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I427" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I427" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J427" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="K427" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B428" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C428" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D428" s="0" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="E428" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F428" s="0" t="s">
-        <v>484</v>
+        <v>452</v>
       </c>
       <c r="G428" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H428" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I428" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I428" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J428" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="K428" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B429" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C429" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D429" s="0" t="s">
         <v>489</v>
       </c>
-      <c r="C429" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D429" s="0" t="s">
-        <v>490</v>
-      </c>
       <c r="E429" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="F429" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G429" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H429" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I429" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I429" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J429" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="K429" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B430" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C430" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D430" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E430" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="F430" s="0" t="s">
-        <v>453</v>
+        <v>483</v>
       </c>
       <c r="G430" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H430" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="I430" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="I430" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="J430" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="K430" s="0" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B431" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="C431" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D431" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E431" s="0" t="s">
-        <v>497</v>
-      </c>
-      <c r="F431" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="G431" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H431" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="I431" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="J431" s="0" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B437" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="K431" s="0" t="s">
-        <v>465</v>
+      <c r="H437" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I437" s="8" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B438" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="H438" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="H438" s="7" t="s">
+      <c r="I438" s="8" t="s">
         <v>500</v>
-      </c>
-      <c r="I438" s="8" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B439" s="0" t="s">
         <v>502</v>
       </c>
-      <c r="H439" s="7" t="s">
+      <c r="H439" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="I439" s="0" t="s">
         <v>500</v>
       </c>
-      <c r="I439" s="8" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B440" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="H440" s="0" t="s">
+    </row>
+    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B442" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="I440" s="0" t="s">
-        <v>501</v>
+      <c r="H442" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="I442" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B443" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="H443" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="H443" s="9" t="s">
-        <v>506</v>
       </c>
       <c r="I443" s="8" t="s">
         <v>41</v>
@@ -7134,7 +7109,7 @@
         <v>507</v>
       </c>
       <c r="H444" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I444" s="8" t="s">
         <v>41</v>
@@ -7145,7 +7120,7 @@
         <v>508</v>
       </c>
       <c r="H445" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I445" s="8" t="s">
         <v>41</v>
@@ -7156,7 +7131,7 @@
         <v>509</v>
       </c>
       <c r="H446" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I446" s="8" t="s">
         <v>41</v>
@@ -7167,7 +7142,7 @@
         <v>510</v>
       </c>
       <c r="H447" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I447" s="8" t="s">
         <v>41</v>
@@ -7178,7 +7153,7 @@
         <v>511</v>
       </c>
       <c r="H448" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I448" s="8" t="s">
         <v>41</v>
@@ -7189,7 +7164,7 @@
         <v>512</v>
       </c>
       <c r="H449" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I449" s="8" t="s">
         <v>41</v>
@@ -7200,7 +7175,7 @@
         <v>513</v>
       </c>
       <c r="H450" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I450" s="8" t="s">
         <v>41</v>
@@ -7211,7 +7186,7 @@
         <v>514</v>
       </c>
       <c r="H451" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I451" s="8" t="s">
         <v>41</v>
@@ -7222,7 +7197,7 @@
         <v>515</v>
       </c>
       <c r="H452" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I452" s="8" t="s">
         <v>41</v>
@@ -7233,1001 +7208,1022 @@
         <v>516</v>
       </c>
       <c r="H453" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I453" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B454" s="0" t="s">
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B456" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="H454" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="I454" s="8" t="s">
-        <v>41</v>
+      <c r="C456" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D456" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="E456" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="F456" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="G456" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H456" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="I456" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J456" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="K456" s="0" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B457" s="0" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="C457" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D457" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G457" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H457" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I457" s="0" t="s">
         <v>24</v>
       </c>
       <c r="J457" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="K457" s="0" t="s">
         <v>522</v>
       </c>
-      <c r="K457" s="0" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B458" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="C458" s="0" t="n">
+    </row>
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B459" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C459" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D458" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="E458" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="F458" s="0" t="s">
-        <v>456</v>
-      </c>
-      <c r="G458" s="0" t="n">
+      <c r="D459" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="E459" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="F459" s="10" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="G459" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H458" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="I458" s="0" t="s">
+      <c r="H459" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="I459" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="J458" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="K458" s="0" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B460" s="0" t="s">
-        <v>527</v>
-      </c>
-      <c r="C460" s="0" t="n">
+      <c r="J459" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="K459" s="0" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B461" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="C461" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D460" s="0" t="s">
-        <v>528</v>
-      </c>
-      <c r="E460" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="F460" s="10" t="n">
-        <v>1E-009</v>
-      </c>
-      <c r="G460" s="0" t="n">
+      <c r="D461" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="E461" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="F461" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="G461" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H460" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="I460" s="0" t="s">
+      <c r="H461" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="I461" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="J460" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="K460" s="0" t="s">
-        <v>523</v>
+      <c r="J461" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="K461" s="0" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B462" s="0" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="C462" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D462" s="0" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E462" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="F462" s="0" t="s">
         <v>534</v>
-      </c>
-      <c r="F462" s="0" t="s">
-        <v>535</v>
       </c>
       <c r="G462" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H462" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I462" s="0" t="s">
         <v>24</v>
       </c>
       <c r="J462" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="K462" s="0" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B463" s="0" t="s">
-        <v>537</v>
-      </c>
-      <c r="C463" s="0" t="n">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B464" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C464" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D463" s="0" t="s">
-        <v>533</v>
-      </c>
-      <c r="E463" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="F463" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="G463" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H463" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="I463" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J463" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="K463" s="0" t="s">
-        <v>523</v>
+      <c r="D464" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E464" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="F464" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="G464" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H464" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="I464" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="J464" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K464" s="0" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B465" s="0" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C465" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D465" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E465" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F465" s="0" t="s">
         <v>541</v>
       </c>
-      <c r="F465" s="0" t="s">
+      <c r="G465" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="G465" s="0" t="s">
-        <v>543</v>
-      </c>
       <c r="H465" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="I465" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I465" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J465" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K465" s="0" t="s">
         <v>546</v>
-      </c>
-      <c r="K465" s="0" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B466" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="C466" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D466" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="F466" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="G466" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="G466" s="0" t="s">
+      <c r="H466" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H466" s="0" t="s">
-        <v>550</v>
-      </c>
       <c r="I466" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J466" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="K466" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B467" s="0" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="C467" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D467" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E467" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="F467" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="F467" s="0" t="s">
-        <v>554</v>
-      </c>
       <c r="G467" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H467" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="I467" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I467" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J467" s="0" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="K467" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B468" s="0" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="C468" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D468" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>557</v>
-      </c>
-      <c r="F468" s="0" t="s">
-        <v>554</v>
+        <v>560</v>
+      </c>
+      <c r="F468" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G468" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H468" s="0" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="I468" s="0" t="s">
-        <v>545</v>
+        <v>562</v>
       </c>
       <c r="J468" s="0" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="K468" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B469" s="0" t="s">
-        <v>560</v>
+        <v>139</v>
       </c>
       <c r="C469" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D469" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F469" s="0" t="n">
-        <v>1</v>
+        <v>564</v>
+      </c>
+      <c r="F469" s="0" t="s">
+        <v>462</v>
       </c>
       <c r="G469" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H469" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H469" s="0" t="s">
-        <v>562</v>
-      </c>
       <c r="I469" s="0" t="s">
-        <v>563</v>
+        <v>544</v>
       </c>
       <c r="J469" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="K469" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B470" s="0" t="s">
-        <v>139</v>
+        <v>566</v>
       </c>
       <c r="C470" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D470" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G470" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H470" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H470" s="0" t="s">
+      <c r="I470" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I470" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J470" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="K470" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B471" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C471" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D471" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>463</v>
+        <v>483</v>
       </c>
       <c r="G471" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H471" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="I471" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I471" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J471" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="K471" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B472" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C472" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D472" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G472" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H472" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H472" s="0" t="s">
-        <v>550</v>
-      </c>
       <c r="I472" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J472" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="K472" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B473" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C473" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D473" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G473" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H473" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="I473" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I473" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J473" s="0" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="K473" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B474" s="0" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="C474" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D474" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G474" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H474" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H474" s="0" t="s">
-        <v>578</v>
-      </c>
       <c r="I474" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J474" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="K474" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B475" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C475" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D475" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G475" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H475" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H475" s="0" t="s">
+      <c r="I475" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I475" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J475" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="K475" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B476" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C476" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D476" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>584</v>
-      </c>
-      <c r="F476" s="0" t="s">
-        <v>484</v>
+        <v>586</v>
+      </c>
+      <c r="F476" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G476" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H476" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H476" s="0" t="s">
+      <c r="I476" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I476" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J476" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="K476" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B477" s="0" t="s">
-        <v>586</v>
+        <v>234</v>
       </c>
       <c r="C477" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D477" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="F477" s="0" t="n">
-        <v>1</v>
+        <v>588</v>
+      </c>
+      <c r="F477" s="0" t="s">
+        <v>483</v>
       </c>
       <c r="G477" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H477" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="I477" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I477" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J477" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="K477" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B478" s="0" t="s">
-        <v>234</v>
+        <v>590</v>
       </c>
       <c r="C478" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D478" s="0" t="s">
-        <v>454</v>
+        <v>591</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>589</v>
-      </c>
-      <c r="F478" s="0" t="s">
-        <v>484</v>
+        <v>592</v>
+      </c>
+      <c r="F478" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G478" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H478" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H478" s="0" t="s">
-        <v>550</v>
-      </c>
       <c r="I478" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J478" s="0" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="K478" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B479" s="0" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="C479" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D479" s="0" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F479" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G479" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H479" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H479" s="0" t="s">
+      <c r="I479" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I479" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J479" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="K479" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B480" s="0" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C480" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D480" s="0" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="F480" s="0" t="n">
-        <v>1</v>
+        <v>599</v>
+      </c>
+      <c r="F480" s="0" t="s">
+        <v>600</v>
       </c>
       <c r="G480" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H480" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H480" s="0" t="s">
+      <c r="I480" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I480" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J480" s="0" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="K480" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B481" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="C481" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D481" s="0" t="s">
-        <v>599</v>
+        <v>453</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="G481" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H481" s="0" t="s">
         <v>543</v>
       </c>
-      <c r="H481" s="0" t="s">
+      <c r="I481" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="I481" s="0" t="s">
-        <v>545</v>
-      </c>
       <c r="J481" s="0" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="K481" s="0" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B482" s="0" t="s">
-        <v>603</v>
-      </c>
-      <c r="C482" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D482" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E482" s="0" t="s">
-        <v>604</v>
-      </c>
-      <c r="F482" s="0" t="s">
-        <v>605</v>
-      </c>
-      <c r="G482" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H482" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="I482" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="J482" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B483" s="0" t="s">
         <v>606</v>
       </c>
-      <c r="K482" s="0" t="s">
-        <v>547</v>
+      <c r="C483" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D483" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E483" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="F483" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="G483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H483" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I483" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J483" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="K483" s="0" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B484" s="0" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="C484" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D484" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D484" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E484" s="0" t="s">
+        <v>613</v>
+      </c>
+      <c r="F484" s="0" t="s">
         <v>608</v>
-      </c>
-      <c r="F484" s="0" t="s">
-        <v>609</v>
       </c>
       <c r="G484" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H484" s="0" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="I484" s="0" t="s">
         <v>20</v>
       </c>
       <c r="J484" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="K484" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="K484" s="0" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B485" s="0" t="s">
-        <v>613</v>
-      </c>
-      <c r="C485" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D485" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E485" s="0" t="s">
-        <v>614</v>
-      </c>
-      <c r="F485" s="0" t="s">
-        <v>609</v>
-      </c>
-      <c r="G485" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H485" s="0" t="s">
-        <v>615</v>
-      </c>
-      <c r="I485" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J485" s="0" t="s">
+    </row>
+    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B487" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="K485" s="0" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B488" s="0" t="s">
+      <c r="C487" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D487" s="0" t="s">
         <v>617</v>
       </c>
-      <c r="C488" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D488" s="0" t="s">
+      <c r="E487" s="0" t="s">
         <v>618</v>
       </c>
-      <c r="E488" s="0" t="s">
+      <c r="F487" s="0" t="s">
         <v>619</v>
       </c>
-      <c r="F488" s="0" t="s">
+      <c r="G487" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H487" s="0" t="s">
         <v>620</v>
       </c>
-      <c r="G488" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H488" s="0" t="s">
+      <c r="I487" s="0" t="s">
         <v>621</v>
       </c>
-      <c r="I488" s="0" t="s">
+      <c r="J487" s="0" t="s">
         <v>622</v>
       </c>
-      <c r="J488" s="0" t="s">
+      <c r="K487" s="0" t="s">
         <v>623</v>
       </c>
-      <c r="K488" s="0" t="s">
+    </row>
+    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B489" s="0" t="s">
         <v>624</v>
+      </c>
+      <c r="C489" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D489" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="E489" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="F489" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="G489" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H489" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="I489" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="J489" s="0" t="s">
+        <v>628</v>
+      </c>
+      <c r="K489" s="0" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B490" s="0" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="C490" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D490" s="0" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>627</v>
-      </c>
-      <c r="F490" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="F490" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G490" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H490" s="0" t="s">
         <v>620</v>
       </c>
-      <c r="G490" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H490" s="0" t="s">
-        <v>628</v>
-      </c>
       <c r="I490" s="0" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J490" s="0" t="s">
+        <v>633</v>
+      </c>
+      <c r="K490" s="0" t="s">
         <v>629</v>
-      </c>
-      <c r="K490" s="0" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B491" s="0" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C491" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D491" s="0" t="s">
-        <v>632</v>
+        <v>453</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>633</v>
-      </c>
-      <c r="F491" s="0" t="n">
-        <v>1</v>
+        <v>635</v>
+      </c>
+      <c r="F491" s="0" t="s">
+        <v>462</v>
       </c>
       <c r="G491" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H491" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="I491" s="0" t="s">
         <v>621</v>
       </c>
-      <c r="I491" s="0" t="s">
+      <c r="J491" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="K491" s="0" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B493" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="C493" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D493" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="E493" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="F493" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="G493" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H493" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="I493" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="J493" s="0" t="s">
         <v>622</v>
       </c>
-      <c r="J491" s="0" t="s">
-        <v>634</v>
-      </c>
-      <c r="K491" s="0" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B492" s="0" t="s">
-        <v>635</v>
-      </c>
-      <c r="C492" s="0" t="n">
+      <c r="K493" s="0" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B497" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="C497" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D492" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E492" s="0" t="s">
-        <v>636</v>
-      </c>
-      <c r="F492" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="G492" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H492" s="0" t="s">
-        <v>621</v>
-      </c>
-      <c r="I492" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="J492" s="0" t="s">
-        <v>637</v>
-      </c>
-      <c r="K492" s="0" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B494" s="0" t="s">
-        <v>617</v>
-      </c>
-      <c r="C494" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D494" s="0" t="s">
-        <v>639</v>
-      </c>
-      <c r="E494" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="F494" s="0" t="s">
-        <v>620</v>
-      </c>
-      <c r="G494" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H494" s="0" t="s">
-        <v>621</v>
-      </c>
-      <c r="I494" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="J494" s="0" t="s">
-        <v>623</v>
-      </c>
-      <c r="K494" s="0" t="s">
-        <v>624</v>
+      <c r="D497" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E497" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="F497" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="G497" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H497" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="I497" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="J497" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="K497" s="0" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B498" s="0" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="C498" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D498" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>642</v>
+        <v>462</v>
       </c>
       <c r="G498" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H498" s="0" t="s">
         <v>148</v>
@@ -8236,126 +8232,126 @@
         <v>349</v>
       </c>
       <c r="J498" s="0" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="K498" s="0" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B499" s="0" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="C499" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D499" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>463</v>
+        <v>650</v>
       </c>
       <c r="G499" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H499" s="0" t="s">
-        <v>148</v>
+        <v>651</v>
       </c>
       <c r="I499" s="0" t="s">
-        <v>349</v>
+        <v>652</v>
       </c>
       <c r="J499" s="0" t="s">
+        <v>653</v>
+      </c>
+      <c r="K499" s="0" t="s">
         <v>647</v>
-      </c>
-      <c r="K499" s="0" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B500" s="0" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="C500" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D500" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E500" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="F500" s="0" t="s">
         <v>650</v>
       </c>
-      <c r="F500" s="0" t="s">
-        <v>651</v>
-      </c>
       <c r="G500" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H500" s="0" t="s">
-        <v>652</v>
+        <v>148</v>
       </c>
       <c r="I500" s="0" t="s">
-        <v>653</v>
+        <v>349</v>
       </c>
       <c r="J500" s="0" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="K500" s="0" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B501" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="C501" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D501" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E501" s="0" t="s">
-        <v>656</v>
-      </c>
-      <c r="F501" s="0" t="s">
-        <v>651</v>
-      </c>
-      <c r="G501" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H501" s="0" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B502" s="0" t="s">
+        <v>657</v>
+      </c>
+      <c r="C502" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D502" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="E502" s="0" t="s">
+        <v>658</v>
+      </c>
+      <c r="F502" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="G502" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H502" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="I501" s="0" t="s">
+      <c r="I502" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="J501" s="0" t="s">
-        <v>657</v>
-      </c>
-      <c r="K501" s="0" t="s">
-        <v>648</v>
+      <c r="J502" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="K502" s="0" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B503" s="0" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C503" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D503" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G503" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H503" s="0" t="s">
         <v>148</v>
@@ -8364,30 +8360,30 @@
         <v>349</v>
       </c>
       <c r="J503" s="0" t="s">
-        <v>643</v>
+        <v>662</v>
       </c>
       <c r="K503" s="0" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B504" s="0" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="C504" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D504" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G504" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H504" s="0" t="s">
         <v>148</v>
@@ -8396,30 +8392,30 @@
         <v>349</v>
       </c>
       <c r="J504" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="K504" s="0" t="s">
         <v>663</v>
-      </c>
-      <c r="K504" s="0" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B505" s="0" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C505" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D505" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G505" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H505" s="0" t="s">
         <v>148</v>
@@ -8428,30 +8424,30 @@
         <v>349</v>
       </c>
       <c r="J505" s="0" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="K505" s="0" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B506" s="0" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="C506" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D506" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="F506" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G506" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H506" s="0" t="s">
         <v>148</v>
@@ -8460,30 +8456,30 @@
         <v>349</v>
       </c>
       <c r="J506" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="K506" s="0" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B507" s="0" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="C507" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D507" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E507" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="F507" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G507" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H507" s="0" t="s">
         <v>148</v>
@@ -8492,30 +8488,30 @@
         <v>349</v>
       </c>
       <c r="J507" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="K507" s="0" t="s">
-        <v>664</v>
+        <v>676</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B508" s="0" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="C508" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D508" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E508" s="0" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="F508" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G508" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H508" s="0" t="s">
         <v>148</v>
@@ -8524,187 +8520,189 @@
         <v>349</v>
       </c>
       <c r="J508" s="0" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="K508" s="0" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B509" s="0" t="s">
-        <v>678</v>
-      </c>
-      <c r="C509" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D509" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E509" s="0" t="s">
-        <v>679</v>
-      </c>
-      <c r="F509" s="0" t="s">
-        <v>642</v>
-      </c>
-      <c r="G509" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H509" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="I509" s="0" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B510" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="C510" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D510" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="E510" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="G510" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H510" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="I510" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="J510" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="K510" s="0" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B514" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="C514" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D514" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="E514" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F514" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="G514" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H514" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="I514" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="J509" s="0" t="s">
-        <v>680</v>
-      </c>
-      <c r="K509" s="0" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B511" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="C511" s="0" t="n">
+      <c r="J514" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="K514" s="0" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B516" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="C516" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D511" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="E511" s="0" t="s">
-        <v>684</v>
-      </c>
-      <c r="G511" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H511" s="0" t="s">
-        <v>685</v>
-      </c>
-      <c r="I511" s="0" t="s">
-        <v>686</v>
-      </c>
-      <c r="J511" s="0" t="s">
-        <v>687</v>
-      </c>
-      <c r="K511" s="0" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B515" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="C515" s="0" t="n">
+      <c r="D516" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="E516" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="F516" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D515" s="0" t="s">
-        <v>690</v>
-      </c>
-      <c r="E515" s="0" t="s">
-        <v>691</v>
-      </c>
-      <c r="F515" s="0" t="s">
-        <v>609</v>
-      </c>
-      <c r="G515" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H515" s="0" t="s">
-        <v>692</v>
-      </c>
-      <c r="I515" s="0" t="s">
+      <c r="G516" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H516" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="I516" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="J515" s="0" t="s">
-        <v>693</v>
-      </c>
-      <c r="K515" s="0" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B517" s="0" t="s">
-        <v>694</v>
-      </c>
-      <c r="C517" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D517" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E517" s="0" t="s">
-        <v>695</v>
-      </c>
-      <c r="F517" s="0" t="s">
-        <v>642</v>
-      </c>
-      <c r="G517" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H517" s="0" t="s">
+      <c r="J516" s="0" t="s">
         <v>696</v>
       </c>
-      <c r="I517" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="J517" s="0" t="s">
+      <c r="K516" s="0" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B519" s="0" t="s">
         <v>697</v>
       </c>
-      <c r="K517" s="0" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B518" s="0" t="s">
+      <c r="C519" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D519" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="E519" s="0" t="s">
         <v>698</v>
       </c>
-      <c r="C518" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D518" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E518" s="0" t="s">
+      <c r="F519" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="G519" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H519" s="3" t="s">
         <v>699</v>
       </c>
-      <c r="F518" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G518" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H518" s="0" t="s">
+      <c r="I519" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J519" s="0" t="s">
         <v>700</v>
       </c>
-      <c r="I518" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="J518" s="0" t="s">
+      <c r="K519" s="0" t="s">
         <v>701</v>
       </c>
-      <c r="K518" s="0" t="s">
-        <v>660</v>
+    </row>
+    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B520" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="C520" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D520" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="E520" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="F520" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="G520" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590daf66-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H520" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="I520" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J520" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="K520" s="0" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B521" s="0" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="C521" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D521" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G521" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e.html","web")</f>
         <v>web</v>
       </c>
       <c r="H521" s="3" t="s">
@@ -8714,736 +8712,672 @@
         <v>41</v>
       </c>
       <c r="J521" s="0" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="K521" s="0" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B522" s="0" t="s">
-        <v>707</v>
-      </c>
-      <c r="C522" s="0" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B524" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="C524" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D524" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="E524" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="F524" s="0" t="s">
+        <v>711</v>
+      </c>
+      <c r="G524" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H524" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="I524" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="J524" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="K524" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B525" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="C525" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D525" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D522" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="E522" s="0" t="s">
-        <v>708</v>
-      </c>
-      <c r="F522" s="0" t="s">
-        <v>456</v>
-      </c>
-      <c r="G522" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590daf66-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H522" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="I522" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J522" s="0" t="s">
-        <v>710</v>
-      </c>
-      <c r="K522" s="0" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B523" s="0" t="s">
-        <v>711</v>
-      </c>
-      <c r="C523" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D523" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="E523" s="0" t="s">
+      <c r="E525" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="F525" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="G525" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H525" s="0" t="s">
         <v>712</v>
       </c>
-      <c r="F523" s="0" t="s">
-        <v>456</v>
-      </c>
-      <c r="G523" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H523" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="I523" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J523" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="K523" s="0" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B526" s="0" t="s">
-        <v>714</v>
-      </c>
-      <c r="C526" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D526" s="0" t="s">
-        <v>482</v>
-      </c>
-      <c r="E526" s="0" t="s">
-        <v>715</v>
-      </c>
-      <c r="F526" s="0" t="s">
-        <v>716</v>
-      </c>
-      <c r="G526" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H526" s="0" t="s">
+      <c r="I525" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="J525" s="0" t="s">
         <v>717</v>
       </c>
-      <c r="I526" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="J526" s="0" t="s">
+      <c r="K525" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B529" s="0" t="s">
         <v>718</v>
       </c>
-      <c r="K526" s="0" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B527" s="0" t="s">
+      <c r="C529" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D529" s="0" t="s">
         <v>719</v>
       </c>
-      <c r="C527" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D527" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E527" s="0" t="s">
+      <c r="E529" s="0" t="s">
         <v>720</v>
       </c>
-      <c r="F527" s="0" t="s">
+      <c r="F529" s="0" t="s">
         <v>721</v>
       </c>
-      <c r="G527" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="H527" s="0" t="s">
-        <v>717</v>
-      </c>
-      <c r="I527" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="J527" s="0" t="s">
-        <v>722</v>
-      </c>
-      <c r="K527" s="0" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B531" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="C531" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D531" s="0" t="s">
-        <v>724</v>
-      </c>
-      <c r="E531" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="F531" s="0" t="s">
-        <v>726</v>
-      </c>
-      <c r="G531" s="0" t="str">
+      <c r="G529" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H531" s="0" t="s">
+      <c r="H529" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="I529" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J529" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="K529" s="0" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B530" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="C530" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D530" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="E530" s="0" t="s">
         <v>727</v>
       </c>
-      <c r="I531" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J531" s="0" t="s">
+      <c r="F530" s="0" t="s">
         <v>728</v>
       </c>
-      <c r="K531" s="0" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B532" s="0" t="s">
-        <v>730</v>
-      </c>
-      <c r="C532" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D532" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="E532" s="0" t="s">
-        <v>732</v>
-      </c>
-      <c r="F532" s="0" t="s">
-        <v>733</v>
-      </c>
-      <c r="G532" s="0" t="str">
+      <c r="G530" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ddf060894b16cf89e906ecfedbba4ffb.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H532" s="0" t="s">
-        <v>727</v>
-      </c>
-      <c r="I532" s="0" t="s">
+      <c r="H530" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="I530" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J532" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="K532" s="0" t="s">
+      <c r="J530" s="0" t="s">
         <v>729</v>
+      </c>
+      <c r="K530" s="0" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="534" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B534" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C534" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D534" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="E534" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="F534" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="G534" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H534" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="I534" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J534" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="K534" s="3" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="536" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B536" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C536" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D536" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E536" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="C536" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D536" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="E536" s="3" t="s">
-        <v>736</v>
-      </c>
       <c r="F536" s="3" t="s">
-        <v>535</v>
+        <v>462</v>
       </c>
       <c r="G536" s="3" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H536" s="3" t="s">
-        <v>737</v>
-      </c>
-      <c r="I536" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J536" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="K536" s="3" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="538" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B538" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="C538" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D538" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="E538" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="F538" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="G538" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H538" s="0" t="s">
+      <c r="H536" s="0" t="s">
+        <v>736</v>
+      </c>
+      <c r="I536" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="J536" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="K536" s="3" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B538" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="C538" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D538" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E538" s="0" t="s">
         <v>741</v>
       </c>
-      <c r="I538" s="0" t="s">
-        <v>742</v>
-      </c>
-      <c r="J538" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="K538" s="3" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B540" s="0" t="s">
-        <v>745</v>
-      </c>
-      <c r="C540" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D540" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E540" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="F540" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="G540" s="0" t="str">
+      <c r="F538" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="G538" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H540" s="0" t="s">
+      <c r="H538" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="I538" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J538" s="0" t="s">
+        <v>743</v>
+      </c>
+      <c r="K538" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="B541" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="C541" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D541" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="E541" s="0" t="s">
         <v>747</v>
       </c>
-      <c r="I540" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J540" s="0" t="s">
+      <c r="F541" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="G541" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124a0cc-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H541" s="0" t="s">
         <v>748</v>
       </c>
-      <c r="K540" s="0" t="s">
-        <v>547</v>
+      <c r="I541" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J541" s="0" t="s">
+        <v>749</v>
+      </c>
+      <c r="K541" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="B542" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="C542" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D542" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="E542" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="F542" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="G542" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124996a-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H542" s="0" t="s">
+        <v>753</v>
+      </c>
+      <c r="I542" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J542" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="K542" s="0" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="0" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="B543" s="0" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="C543" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D543" s="0" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="E543" s="0" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>620</v>
+        <v>483</v>
       </c>
       <c r="G543" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124a0cc-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/71249bb8-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H543" s="0" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="I543" s="0" t="s">
         <v>50</v>
       </c>
       <c r="J543" s="0" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="K543" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="0" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="B544" s="0" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="C544" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D544" s="0" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="E544" s="0" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="F544" s="0" t="s">
-        <v>757</v>
+        <v>619</v>
       </c>
       <c r="G544" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124996a-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124926c-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H544" s="0" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="I544" s="0" t="s">
         <v>50</v>
       </c>
       <c r="J544" s="0" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="K544" s="0" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A545" s="0" t="s">
-        <v>749</v>
-      </c>
-      <c r="B545" s="0" t="s">
-        <v>760</v>
-      </c>
-      <c r="C545" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A548" s="0" t="s">
+        <v>763</v>
+      </c>
+      <c r="B548" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="C548" s="0" t="s">
+        <v>765</v>
+      </c>
+      <c r="D548" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D545" s="0" t="s">
-        <v>751</v>
-      </c>
-      <c r="E545" s="0" t="s">
-        <v>761</v>
-      </c>
-      <c r="F545" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="G545" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/71249bb8-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H545" s="0" t="s">
-        <v>762</v>
-      </c>
-      <c r="I545" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J545" s="0" t="s">
-        <v>763</v>
-      </c>
-      <c r="K545" s="0" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A546" s="0" t="s">
-        <v>749</v>
-      </c>
-      <c r="B546" s="0" t="s">
-        <v>764</v>
-      </c>
-      <c r="C546" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D546" s="0" t="s">
-        <v>751</v>
-      </c>
-      <c r="E546" s="0" t="s">
-        <v>765</v>
-      </c>
-      <c r="F546" s="0" t="s">
-        <v>620</v>
-      </c>
-      <c r="G546" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124926c-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H546" s="0" t="s">
+      <c r="E548" s="0" t="s">
         <v>766</v>
       </c>
-      <c r="I546" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J546" s="0" t="s">
-        <v>767</v>
-      </c>
-      <c r="K546" s="0" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A550" s="0" t="s">
-        <v>768</v>
-      </c>
-      <c r="B550" s="0" t="s">
-        <v>769</v>
-      </c>
-      <c r="C550" s="0" t="s">
-        <v>770</v>
-      </c>
-      <c r="D550" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E550" s="0" t="s">
-        <v>771</v>
-      </c>
-      <c r="F550" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="G550" s="0" t="str">
+      <c r="F548" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="G548" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/67adc30ae1278d2ef6d696ba0e2c92e8.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H550" s="11" t="s">
+      <c r="H548" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="I548" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="J548" s="0" t="s">
+        <v>769</v>
+      </c>
+      <c r="K548" s="0" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A549" s="0" t="s">
+        <v>763</v>
+      </c>
+      <c r="B549" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="C549" s="0" t="s">
         <v>772</v>
       </c>
-      <c r="I550" s="11" t="s">
+      <c r="D549" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E549" s="0" t="s">
         <v>773</v>
       </c>
-      <c r="J550" s="0" t="s">
+      <c r="F549" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="G549" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d421b6923b396998106a8c1c66ea07f1.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H549" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="I549" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="J549" s="0" t="s">
         <v>774</v>
       </c>
-      <c r="K550" s="0" t="s">
-        <v>775</v>
+      <c r="K549" s="0" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="B551" s="0" t="s">
         <v>776</v>
       </c>
       <c r="C551" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D551" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E551" s="0" t="s">
         <v>777</v>
       </c>
-      <c r="D551" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E551" s="0" t="s">
+      <c r="F551" s="0" t="s">
+        <v>711</v>
+      </c>
+      <c r="G551" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/069ed8a3f93e92dab9e61f59b4d5338e.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H551" s="3" t="s">
         <v>778</v>
       </c>
-      <c r="F551" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="G551" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d421b6923b396998106a8c1c66ea07f1.html","web")</f>
+      <c r="I551" s="0" t="s">
+        <v>779</v>
+      </c>
+      <c r="J551" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="K551" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A552" s="0" t="s">
+        <v>775</v>
+      </c>
+      <c r="B552" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C552" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D552" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E552" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="F552" s="0" t="s">
+        <v>783</v>
+      </c>
+      <c r="G552" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f946653cd518e221676f263a895c7852.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H551" s="11" t="s">
-        <v>772</v>
-      </c>
-      <c r="I551" s="11" t="s">
-        <v>773</v>
-      </c>
-      <c r="J551" s="0" t="s">
+      <c r="H552" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="I552" s="0" t="s">
         <v>779</v>
       </c>
-      <c r="K551" s="0" t="s">
-        <v>775</v>
+      <c r="J552" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="K552" s="0" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="0" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="B553" s="0" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
       <c r="C553" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D553" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D553" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E553" s="0" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="F553" s="0" t="s">
-        <v>716</v>
+        <v>483</v>
       </c>
       <c r="G553" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/069ed8a3f93e92dab9e61f59b4d5338e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H553" s="11" t="s">
-        <v>783</v>
+      <c r="H553" s="3" t="s">
+        <v>788</v>
       </c>
       <c r="I553" s="0" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="J553" s="0" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="K553" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="B554" s="0" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
       <c r="C554" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D554" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D554" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="E554" s="0" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="F554" s="0" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="G554" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f946653cd518e221676f263a895c7852.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H554" s="11" t="s">
+      <c r="H554" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="I554" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="I554" s="0" t="s">
-        <v>784</v>
-      </c>
       <c r="J554" s="0" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="K554" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="0" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="B555" s="0" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="C555" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D555" s="0" t="s">
-        <v>454</v>
+        <v>489</v>
       </c>
       <c r="E555" s="0" t="s">
-        <v>792</v>
+        <v>490</v>
       </c>
       <c r="F555" s="0" t="s">
-        <v>484</v>
+        <v>452</v>
       </c>
       <c r="G555" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cbf-4d35-11e8-be0a-1c4d70487308.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H555" s="11" t="s">
-        <v>793</v>
+      <c r="H555" s="3" t="s">
+        <v>796</v>
       </c>
       <c r="I555" s="0" t="s">
-        <v>794</v>
+        <v>17</v>
       </c>
       <c r="J555" s="0" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="K555" s="0" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A556" s="0" t="s">
-        <v>780</v>
-      </c>
-      <c r="B556" s="0" t="s">
-        <v>796</v>
-      </c>
-      <c r="C556" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D556" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E556" s="0" t="s">
-        <v>797</v>
-      </c>
-      <c r="F556" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="G556" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H556" s="11" t="s">
-        <v>798</v>
-      </c>
-      <c r="I556" s="0" t="s">
-        <v>794</v>
-      </c>
-      <c r="J556" s="0" t="s">
-        <v>799</v>
-      </c>
-      <c r="K556" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="0" t="s">
-        <v>780</v>
+        <v>798</v>
       </c>
       <c r="B557" s="0" t="s">
+        <v>799</v>
+      </c>
+      <c r="C557" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D557" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="E557" s="0" t="s">
         <v>800</v>
       </c>
-      <c r="C557" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D557" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E557" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="F557" s="0" t="s">
-        <v>453</v>
-      </c>
       <c r="G557" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cbf-4d35-11e8-be0a-1c4d70487308.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/962e51dc-267b-11e7-96a5-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H557" s="11" t="s">
+      <c r="H557" s="3" t="s">
         <v>801</v>
       </c>
       <c r="I557" s="0" t="s">
         <v>17</v>
       </c>
       <c r="J557" s="0" t="s">
-        <v>802</v>
+        <v>686</v>
       </c>
       <c r="K557" s="0" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A559" s="0" t="s">
-        <v>803</v>
-      </c>
-      <c r="B559" s="0" t="s">
-        <v>804</v>
-      </c>
-      <c r="C559" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="D559" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="E559" s="0" t="s">
-        <v>805</v>
-      </c>
-      <c r="G559" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/962e51dc-267b-11e7-96a5-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H559" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="I559" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J559" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="K559" s="0" t="s">
-        <v>688</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Remove rsutcsaf from the ignored and pre ignored list, because it appeared this variable is already available with PEXTRA #556.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="798">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2151,31 +2151,19 @@
     <t xml:space="preserve">negative log10 of hydrogen ion concentration with the concentration expressed as mol H kg-1.</t>
   </si>
   <si>
-    <t xml:space="preserve">rsutcsaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Outgoing Clear-Sky, Aerosol-Free Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore because part of RFMIP-IRF and we don't participate in that experiment of RFMIP. Moreover grib 128.212-126.068 won't work here, because then accumulated and instantaneous fluxes are mixed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux corresponding to rsutcs resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
+    <t xml:space="preserve">rsdscsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downwelling Clear-Sky, Aerosol-Free Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not available, moreover they can be ignored because part of RFMIP-IRF and we don't participate in that experiment of RFMIP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated in the absence of aerosols and clouds.</t>
   </si>
   <si>
     <t xml:space="preserve">RFMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsdscsaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downwelling Clear-Sky, Aerosol-Free Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not available, moreover they can be ignored because part of RFMIP-IRF and we don't participate in that experiment of RFMIP.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculated in the absence of aerosols and clouds.</t>
   </si>
   <si>
     <t xml:space="preserve">rsuscsaf</t>
@@ -2719,8 +2707,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C369" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A389" activeCellId="0" sqref="A389"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A499" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A519" activeCellId="0" sqref="A519"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8636,7 +8624,7 @@
         <v>455</v>
       </c>
       <c r="G519" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590daf66-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
       <c r="H519" s="3" t="s">
@@ -8669,76 +8657,75 @@
         <v>455</v>
       </c>
       <c r="G520" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590daf66-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e.html","web")</f>
         <v>web</v>
       </c>
       <c r="H520" s="3" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="I520" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J520" s="0" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K520" s="0" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B521" s="0" t="s">
+    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B523" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="C523" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D523" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="E523" s="0" t="s">
         <v>706</v>
       </c>
-      <c r="C521" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="D521" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="E521" s="0" t="s">
+      <c r="F523" s="0" t="s">
         <v>707</v>
       </c>
-      <c r="F521" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="G521" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H521" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="I521" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J521" s="0" t="s">
+      <c r="G523" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="H523" s="0" t="s">
         <v>708</v>
       </c>
-      <c r="K521" s="0" t="s">
-        <v>701</v>
+      <c r="I523" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="J523" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="K523" s="0" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B524" s="0" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C524" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D524" s="0" t="s">
-        <v>481</v>
+        <v>453</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="G524" s="0" t="s">
         <v>542</v>
       </c>
       <c r="H524" s="0" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="I524" s="0" t="s">
         <v>197</v>
@@ -8750,234 +8737,238 @@
         <v>459</v>
       </c>
     </row>
-    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B525" s="0" t="s">
+    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B528" s="0" t="s">
         <v>714</v>
       </c>
-      <c r="C525" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D525" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="E525" s="0" t="s">
+      <c r="C528" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D528" s="0" t="s">
         <v>715</v>
       </c>
-      <c r="F525" s="0" t="s">
+      <c r="E528" s="0" t="s">
         <v>716</v>
       </c>
-      <c r="G525" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="H525" s="0" t="s">
-        <v>712</v>
-      </c>
-      <c r="I525" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="J525" s="0" t="s">
+      <c r="F528" s="0" t="s">
         <v>717</v>
       </c>
-      <c r="K525" s="0" t="s">
-        <v>459</v>
+      <c r="G528" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H528" s="0" t="s">
+        <v>718</v>
+      </c>
+      <c r="I528" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J528" s="0" t="s">
+        <v>719</v>
+      </c>
+      <c r="K528" s="0" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B529" s="0" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="C529" s="0" t="s">
         <v>452</v>
       </c>
       <c r="D529" s="0" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="E529" s="0" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="F529" s="0" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="G529" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ddf060894b16cf89e906ecfedbba4ffb.html","web")</f>
         <v>web</v>
       </c>
       <c r="H529" s="0" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="I529" s="0" t="s">
         <v>17</v>
       </c>
       <c r="J529" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="K529" s="0" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B530" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C530" s="0" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="533" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B533" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="C533" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D530" s="0" t="s">
-        <v>726</v>
-      </c>
-      <c r="E530" s="0" t="s">
+      <c r="D533" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="E533" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="F530" s="0" t="s">
-        <v>728</v>
-      </c>
-      <c r="G530" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ddf060894b16cf89e906ecfedbba4ffb.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H530" s="0" t="s">
-        <v>722</v>
-      </c>
-      <c r="I530" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J530" s="0" t="s">
-        <v>729</v>
-      </c>
-      <c r="K530" s="0" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="534" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B534" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C534" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="D534" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="E534" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="F534" s="3" t="s">
+      <c r="F533" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="G534" s="3" t="str">
+      <c r="G533" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H534" s="3" t="s">
-        <v>732</v>
-      </c>
-      <c r="I534" s="3" t="s">
+      <c r="H533" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="I533" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J534" s="3" t="s">
+      <c r="J533" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="K533" s="3" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="535" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B535" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C535" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D535" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E535" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="K534" s="3" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="536" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B536" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="C536" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="D536" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E536" s="3" t="s">
-        <v>735</v>
-      </c>
-      <c r="F536" s="3" t="s">
+      <c r="F535" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="G536" s="3" t="str">
+      <c r="G535" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H536" s="0" t="s">
+      <c r="H535" s="0" t="s">
+        <v>732</v>
+      </c>
+      <c r="I535" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="J535" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="K535" s="3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B537" s="0" t="s">
         <v>736</v>
       </c>
-      <c r="I536" s="0" t="s">
+      <c r="C537" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D537" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E537" s="0" t="s">
         <v>737</v>
       </c>
-      <c r="J536" s="3" t="s">
-        <v>738</v>
-      </c>
-      <c r="K536" s="3" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B538" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="C538" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="D538" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="E538" s="0" t="s">
-        <v>741</v>
-      </c>
-      <c r="F538" s="0" t="s">
+      <c r="F537" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="G538" s="0" t="str">
+      <c r="G537" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H538" s="0" t="s">
+      <c r="H537" s="0" t="s">
+        <v>738</v>
+      </c>
+      <c r="I537" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J537" s="0" t="s">
+        <v>739</v>
+      </c>
+      <c r="K537" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="B540" s="0" t="s">
+        <v>741</v>
+      </c>
+      <c r="C540" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D540" s="0" t="s">
         <v>742</v>
       </c>
-      <c r="I538" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J538" s="0" t="s">
+      <c r="E540" s="0" t="s">
         <v>743</v>
       </c>
-      <c r="K538" s="0" t="s">
+      <c r="F540" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="G540" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124a0cc-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H540" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="I540" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J540" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="K540" s="0" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="0" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B541" s="0" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C541" s="0" t="s">
         <v>452</v>
       </c>
       <c r="D541" s="0" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="E541" s="0" t="s">
         <v>747</v>
       </c>
       <c r="F541" s="0" t="s">
-        <v>619</v>
+        <v>748</v>
       </c>
       <c r="G541" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124a0cc-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124996a-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H541" s="0" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="I541" s="0" t="s">
         <v>50</v>
       </c>
       <c r="J541" s="0" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="K541" s="0" t="s">
         <v>546</v>
@@ -8985,25 +8976,25 @@
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="0" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B542" s="0" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="C542" s="0" t="s">
         <v>452</v>
       </c>
       <c r="D542" s="0" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="E542" s="0" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="F542" s="0" t="s">
-        <v>752</v>
+        <v>483</v>
       </c>
       <c r="G542" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124996a-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/71249bb8-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H542" s="0" t="s">
@@ -9021,7 +9012,7 @@
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="0" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B543" s="0" t="s">
         <v>755</v>
@@ -9030,16 +9021,16 @@
         <v>452</v>
       </c>
       <c r="D543" s="0" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="E543" s="0" t="s">
         <v>756</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>483</v>
+        <v>619</v>
       </c>
       <c r="G543" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/71249bb8-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124926c-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H543" s="0" t="s">
@@ -9055,120 +9046,120 @@
         <v>546</v>
       </c>
     </row>
-    <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A544" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="B544" s="0" t="s">
+    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A547" s="0" t="s">
         <v>759</v>
       </c>
-      <c r="C544" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="D544" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="E544" s="0" t="s">
+      <c r="B547" s="0" t="s">
         <v>760</v>
       </c>
-      <c r="F544" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="G544" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124926c-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+      <c r="C547" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="D547" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E547" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="F547" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="G547" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/67adc30ae1278d2ef6d696ba0e2c92e8.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H544" s="0" t="s">
-        <v>761</v>
-      </c>
-      <c r="I544" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J544" s="0" t="s">
-        <v>762</v>
-      </c>
-      <c r="K544" s="0" t="s">
-        <v>546</v>
+      <c r="H547" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="I547" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="J547" s="0" t="s">
+        <v>765</v>
+      </c>
+      <c r="K547" s="0" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="0" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B548" s="0" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="C548" s="0" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="D548" s="0" t="s">
         <v>453</v>
       </c>
       <c r="E548" s="0" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="F548" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G548" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/67adc30ae1278d2ef6d696ba0e2c92e8.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H548" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="I548" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="J548" s="0" t="s">
-        <v>769</v>
-      </c>
-      <c r="K548" s="0" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A549" s="0" t="s">
-        <v>763</v>
-      </c>
-      <c r="B549" s="0" t="s">
-        <v>771</v>
-      </c>
-      <c r="C549" s="0" t="s">
-        <v>772</v>
-      </c>
-      <c r="D549" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="E549" s="0" t="s">
-        <v>773</v>
-      </c>
-      <c r="F549" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="G549" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d421b6923b396998106a8c1c66ea07f1.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H549" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="I549" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="J549" s="0" t="s">
+      <c r="H548" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="I548" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="J548" s="0" t="s">
+        <v>770</v>
+      </c>
+      <c r="K548" s="0" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A550" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="B550" s="0" t="s">
+        <v>772</v>
+      </c>
+      <c r="C550" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D550" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E550" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="F550" s="0" t="s">
+        <v>707</v>
+      </c>
+      <c r="G550" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/069ed8a3f93e92dab9e61f59b4d5338e.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H550" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="K549" s="0" t="s">
-        <v>770</v>
+      <c r="I550" s="0" t="s">
+        <v>775</v>
+      </c>
+      <c r="J550" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="K550" s="0" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B551" s="0" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C551" s="0" t="s">
         <v>452</v>
@@ -9177,23 +9168,23 @@
         <v>453</v>
       </c>
       <c r="E551" s="0" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F551" s="0" t="s">
-        <v>711</v>
+        <v>779</v>
       </c>
       <c r="G551" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/069ed8a3f93e92dab9e61f59b4d5338e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f946653cd518e221676f263a895c7852.html","web")</f>
         <v>web</v>
       </c>
       <c r="H551" s="3" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="I551" s="0" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="J551" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="K551" s="0" t="s">
         <v>459</v>
@@ -9201,10 +9192,10 @@
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="0" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B552" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C552" s="0" t="s">
         <v>452</v>
@@ -9213,23 +9204,23 @@
         <v>453</v>
       </c>
       <c r="E552" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="F552" s="0" t="s">
-        <v>783</v>
+        <v>483</v>
       </c>
       <c r="G552" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f946653cd518e221676f263a895c7852.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
         <v>web</v>
       </c>
       <c r="H552" s="3" t="s">
         <v>784</v>
       </c>
       <c r="I552" s="0" t="s">
-        <v>779</v>
+        <v>785</v>
       </c>
       <c r="J552" s="0" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="K552" s="0" t="s">
         <v>459</v>
@@ -9237,10 +9228,10 @@
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="0" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B553" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C553" s="0" t="s">
         <v>452</v>
@@ -9249,20 +9240,20 @@
         <v>453</v>
       </c>
       <c r="E553" s="0" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F553" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G553" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
         <v>web</v>
       </c>
       <c r="H553" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="I553" s="0" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="J553" s="0" t="s">
         <v>790</v>
@@ -9273,7 +9264,7 @@
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B554" s="0" t="s">
         <v>791</v>
@@ -9282,100 +9273,65 @@
         <v>452</v>
       </c>
       <c r="D554" s="0" t="s">
-        <v>453</v>
+        <v>489</v>
       </c>
       <c r="E554" s="0" t="s">
-        <v>792</v>
+        <v>490</v>
       </c>
       <c r="F554" s="0" t="s">
-        <v>483</v>
+        <v>452</v>
       </c>
       <c r="G554" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H554" s="3" t="s">
-        <v>793</v>
-      </c>
-      <c r="I554" s="0" t="s">
-        <v>789</v>
-      </c>
-      <c r="J554" s="0" t="s">
-        <v>794</v>
-      </c>
-      <c r="K554" s="0" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A555" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="B555" s="0" t="s">
-        <v>795</v>
-      </c>
-      <c r="C555" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="D555" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="E555" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="F555" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="G555" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cbf-4d35-11e8-be0a-1c4d70487308.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H555" s="3" t="s">
+      <c r="H554" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="I554" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J554" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="K554" s="0" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="B556" s="0" t="s">
+        <v>795</v>
+      </c>
+      <c r="C556" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D556" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="E556" s="0" t="s">
         <v>796</v>
       </c>
-      <c r="I555" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J555" s="0" t="s">
-        <v>797</v>
-      </c>
-      <c r="K555" s="0" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A557" s="0" t="s">
-        <v>798</v>
-      </c>
-      <c r="B557" s="0" t="s">
-        <v>799</v>
-      </c>
-      <c r="C557" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="D557" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="E557" s="0" t="s">
-        <v>800</v>
-      </c>
-      <c r="G557" s="0" t="str">
+      <c r="G556" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/962e51dc-267b-11e7-96a5-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H557" s="3" t="s">
-        <v>801</v>
-      </c>
-      <c r="I557" s="0" t="s">
+      <c r="H556" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="I556" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J557" s="0" t="s">
+      <c r="J556" s="0" t="s">
         <v>686</v>
       </c>
-      <c r="K557" s="0" t="s">
+      <c r="K556" s="0" t="s">
         <v>687</v>
       </c>
     </row>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>